<commit_message>
Update Excels to match any region
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Facturador-Multiusuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A4A983-B810-488F-AA74-E7D42F96C4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD680BF-2722-4D9A-9832-AD34BA28294E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1213,10 +1213,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A17"/>
+      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1233,8 @@
     <col min="13" max="13" width="9.140625" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" customWidth="1"/>
     <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="26" width="9.140625" customWidth="1"/>
+    <col min="16" max="25" width="9.140625" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" customWidth="1"/>
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" customWidth="1"/>
@@ -1388,19 +1389,19 @@
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f ca="1">TODAY()</f>
-        <v>45051</v>
-      </c>
-      <c r="B2" s="9" t="str">
-        <f t="shared" ref="B2:B17" ca="1" si="0">TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/aaaa")</f>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C2" s="9" t="str">
-        <f t="shared" ref="C2:C17" ca="1" si="1">TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D2" s="9" t="str">
-        <f t="shared" ref="D2:D17" ca="1" si="2">TEXT(A2+14,"dd/mm/aaaa")</f>
-        <v>19/05/2023</v>
+        <v>45108</v>
+      </c>
+      <c r="B2" s="9">
+        <f ca="1">DATE(YEAR(C2),MONTH(C2),1)</f>
+        <v>45078</v>
+      </c>
+      <c r="C2" s="9">
+        <f ca="1">EOMONTH(A2,-1)</f>
+        <v>45107</v>
+      </c>
+      <c r="D2" s="9">
+        <f ca="1">A2+14</f>
+        <v>45122</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -1448,7 +1449,7 @@
         <v>2</v>
       </c>
       <c r="V2" s="18" t="str">
-        <f t="shared" ref="V2:V17" si="3">SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
+        <f t="shared" ref="V2:V17" si="0">SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
         <v>7.003044</v>
       </c>
       <c r="W2" s="18" t="str">
@@ -1456,19 +1457,19 @@
         <v>19000.00</v>
       </c>
       <c r="X2" s="1" t="str">
-        <f t="shared" ref="X2:X17" si="4">TEXT(R2,"00000")</f>
+        <f t="shared" ref="X2:X17" si="1">TEXT(R2,"00000")</f>
         <v>00000</v>
       </c>
       <c r="Y2" s="1" t="str">
-        <f t="shared" ref="Y2:Y17" si="5">TEXT(S2,"00000000")</f>
+        <f t="shared" ref="Y2:Y17" si="2">TEXT(S2,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="Z2" s="1" t="str">
-        <f t="shared" ref="Z2:Z17" si="6">TEXT(T2,"DD/MM/aaaa")</f>
-        <v>00/01/1900</v>
+      <c r="Z2" s="9">
+        <f>T2</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="13">
-        <f t="shared" ref="AA2:AA17" si="7">IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
+        <f t="shared" ref="AA2:AA17" si="3">IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
         <v>27942.15</v>
       </c>
       <c r="AB2" s="13">
@@ -1476,7 +1477,7 @@
         <v>160999.99</v>
       </c>
       <c r="AC2" s="10" t="str">
-        <f t="shared" ref="AC2:AC17" si="8">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
+        <f t="shared" ref="AC2:AC17" si="4">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
         <v>133057.84</v>
       </c>
       <c r="AD2" s="10" t="str">
@@ -1485,7 +1486,7 @@
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1">
-        <f t="shared" ref="AF2:AF17" si="9">ROW(K2)</f>
+        <f t="shared" ref="AF2:AF17" si="5">ROW(K2)</f>
         <v>2</v>
       </c>
       <c r="AG2" s="15" t="str">
@@ -1493,15 +1494,15 @@
         <v>30525390086-1</v>
       </c>
       <c r="AH2" s="1">
-        <f t="shared" ref="AH2:AH17" si="10">IF(K1=K2,1,0)</f>
+        <f t="shared" ref="AH2:AH17" si="6">IF(K1=K2,1,0)</f>
         <v>0</v>
       </c>
       <c r="AI2" s="1">
-        <f t="shared" ref="AI2:AI17" si="11">IF(K2=K3,1,0)</f>
+        <f t="shared" ref="AI2:AI17" si="7">IF(K2=K3,1,0)</f>
         <v>0</v>
       </c>
       <c r="AJ2" s="1" t="str">
-        <f t="shared" ref="AJ2:AJ17" si="12">RIGHT(F2)</f>
+        <f t="shared" ref="AJ2:AJ17" si="8">RIGHT(F2)</f>
         <v>A</v>
       </c>
       <c r="AK2" s="1">
@@ -1514,15 +1515,15 @@
         <v>160999.98000000001</v>
       </c>
       <c r="AN2" s="13">
-        <f t="shared" ref="AN2:AN17" si="13">ROUND((AM2/(1+P2)),2)</f>
+        <f t="shared" ref="AN2:AN17" si="9">ROUND((AM2/(1+P2)),2)</f>
         <v>133057.82999999999</v>
       </c>
       <c r="AO2" s="20">
-        <f t="shared" ref="AO2:AO17" si="14">IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
+        <f t="shared" ref="AO2:AO17" si="10">IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
         <v>7.003044</v>
       </c>
       <c r="AP2" s="13">
-        <f t="shared" ref="AP2:AP17" si="15">IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
+        <f t="shared" ref="AP2:AP17" si="11">IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
         <v>161000</v>
       </c>
       <c r="AQ2" s="20">
@@ -1533,20 +1534,20 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f t="shared" ref="A3:A17" ca="1" si="16">TODAY()</f>
-        <v>45051</v>
-      </c>
-      <c r="B3" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C3" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D3" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ref="A3:A17" ca="1" si="12">TODAY()</f>
+        <v>45108</v>
+      </c>
+      <c r="B3" s="9">
+        <f t="shared" ref="B3:B17" ca="1" si="13">DATE(YEAR(C3),MONTH(C3),1)</f>
+        <v>45078</v>
+      </c>
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:C17" ca="1" si="14">EOMONTH(A3,-1)</f>
+        <v>45107</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" ref="D3:D17" ca="1" si="15">A3+14</f>
+        <v>45122</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1571,7 +1572,7 @@
       </c>
       <c r="L3" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B3,"mmmm"))</f>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Junio</v>
       </c>
       <c r="M3" s="4">
         <v>8.0252280000000003</v>
@@ -1580,7 +1581,7 @@
         <v>19000</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O17" si="17">M3*N3</f>
+        <f t="shared" ref="O3:O17" si="16">M3*N3</f>
         <v>152479.33199999999</v>
       </c>
       <c r="P3" s="11" t="s">
@@ -1595,27 +1596,27 @@
         <v>2</v>
       </c>
       <c r="V3" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>8.025228</v>
+      </c>
+      <c r="W3" s="18" t="str">
+        <f t="shared" ref="W3:W17" si="17">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
+        <v>19000.00</v>
+      </c>
+      <c r="X3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y3" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z3" s="9">
+        <f t="shared" ref="Z3:Z17" si="18">T3</f>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="13">
         <f t="shared" si="3"/>
-        <v>8.025228</v>
-      </c>
-      <c r="W3" s="18" t="str">
-        <f t="shared" ref="W3:W17" si="18">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
-        <v>19000.00</v>
-      </c>
-      <c r="X3" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y3" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z3" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA3" s="13">
-        <f t="shared" si="7"/>
         <v>32020.66</v>
       </c>
       <c r="AB3" s="13">
@@ -1623,7 +1624,7 @@
         <v>184499.99</v>
       </c>
       <c r="AC3" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>152479.33</v>
       </c>
       <c r="AD3" s="10" t="str">
@@ -1632,7 +1633,7 @@
       </c>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="AG3" s="15" t="str">
@@ -1640,15 +1641,15 @@
         <v>30525733870-1</v>
       </c>
       <c r="AH3" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI3" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK3" s="1">
@@ -1661,15 +1662,15 @@
         <v>184499.99</v>
       </c>
       <c r="AN3" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>152479.32999999999</v>
       </c>
       <c r="AO3" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>8.0252280000000003</v>
       </c>
       <c r="AP3" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>184500</v>
       </c>
       <c r="AQ3" s="20">
@@ -1680,20 +1681,20 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B4" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C4" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D4" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B4" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1718,7 +1719,7 @@
       </c>
       <c r="L4" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Junio</v>
       </c>
       <c r="M4" s="4">
         <v>10.004348999999999</v>
@@ -1727,7 +1728,7 @@
         <v>19000</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>190082.63099999999</v>
       </c>
       <c r="P4" s="11" t="s">
@@ -1742,27 +1743,27 @@
         <v>2</v>
       </c>
       <c r="V4" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>10.004349</v>
+      </c>
+      <c r="W4" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z4" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="13">
         <f t="shared" si="3"/>
-        <v>10.004349</v>
-      </c>
-      <c r="W4" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X4" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y4" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z4" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA4" s="13">
-        <f t="shared" si="7"/>
         <v>39917.35</v>
       </c>
       <c r="AB4" s="13">
@@ -1770,7 +1771,7 @@
         <v>229999.98</v>
       </c>
       <c r="AC4" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>190082.63</v>
       </c>
       <c r="AD4" s="10" t="str">
@@ -1779,7 +1780,7 @@
       </c>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="AG4" s="15" t="str">
@@ -1787,15 +1788,15 @@
         <v>30610252334-1</v>
       </c>
       <c r="AH4" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI4" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK4" s="1">
@@ -1808,15 +1809,15 @@
         <v>229999.98</v>
       </c>
       <c r="AN4" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>190082.63</v>
       </c>
       <c r="AO4" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AP4" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>230000</v>
       </c>
       <c r="AQ4" s="20">
@@ -1827,20 +1828,20 @@
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B5" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C5" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D5" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B5" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -1865,7 +1866,7 @@
       </c>
       <c r="L5" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B5,"mmmm"))</f>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Junio</v>
       </c>
       <c r="M5" s="4">
         <v>9.0256629999999998</v>
@@ -1874,7 +1875,7 @@
         <v>19000</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>171487.59700000001</v>
       </c>
       <c r="P5" s="11" t="s">
@@ -1889,27 +1890,27 @@
         <v>2</v>
       </c>
       <c r="V5" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>9.025663</v>
+      </c>
+      <c r="W5" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z5" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="13">
         <f t="shared" si="3"/>
-        <v>9.025663</v>
-      </c>
-      <c r="W5" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X5" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y5" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z5" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA5" s="13">
-        <f t="shared" si="7"/>
         <v>36012.400000000001</v>
       </c>
       <c r="AB5" s="13">
@@ -1917,7 +1918,7 @@
         <v>207500</v>
       </c>
       <c r="AC5" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>171487.60</v>
       </c>
       <c r="AD5" s="10" t="str">
@@ -1926,7 +1927,7 @@
       </c>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AG5" s="15" t="str">
@@ -1934,15 +1935,15 @@
         <v>30710964277-1</v>
       </c>
       <c r="AH5" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI5" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK5" s="1">
@@ -1955,15 +1956,15 @@
         <v>207499.99</v>
       </c>
       <c r="AN5" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>171487.6</v>
       </c>
       <c r="AO5" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>9.0256629999999998</v>
       </c>
       <c r="AP5" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>207500</v>
       </c>
       <c r="AQ5" s="20">
@@ -1974,20 +1975,20 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B6" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C6" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D6" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B6" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -2012,7 +2013,7 @@
       </c>
       <c r="L6" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B6,"mmmm"))</f>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Junio</v>
       </c>
       <c r="M6" s="4">
         <v>5.0239229999999999</v>
@@ -2021,7 +2022,7 @@
         <v>19000</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>95454.536999999997</v>
       </c>
       <c r="P6" s="11" t="s">
@@ -2044,27 +2045,27 @@
         <v>2</v>
       </c>
       <c r="V6" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>5.023923</v>
+      </c>
+      <c r="W6" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000003</v>
+      </c>
+      <c r="Z6" s="9">
+        <f t="shared" si="18"/>
+        <v>44816</v>
+      </c>
+      <c r="AA6" s="13">
         <f t="shared" si="3"/>
-        <v>5.023923</v>
-      </c>
-      <c r="W6" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X6" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00002</v>
-      </c>
-      <c r="Y6" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000003</v>
-      </c>
-      <c r="Z6" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="AA6" s="13">
-        <f t="shared" si="7"/>
         <v>20045.45</v>
       </c>
       <c r="AB6" s="13">
@@ -2072,7 +2073,7 @@
         <v>115499.99</v>
       </c>
       <c r="AC6" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>95454.54</v>
       </c>
       <c r="AD6" s="10" t="str">
@@ -2081,7 +2082,7 @@
       </c>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AG6" s="15" t="str">
@@ -2089,15 +2090,15 @@
         <v>33610006189-1</v>
       </c>
       <c r="AH6" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI6" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ6" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK6" s="1">
@@ -2110,15 +2111,15 @@
         <v>115499.99</v>
       </c>
       <c r="AN6" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>95454.54</v>
       </c>
       <c r="AO6" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>5.0239229999999999</v>
       </c>
       <c r="AP6" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>115500</v>
       </c>
       <c r="AQ6" s="20">
@@ -2129,20 +2130,20 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B7" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C7" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D7" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B7" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2175,7 +2176,7 @@
         <v>19000</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>95041.305999999997</v>
       </c>
       <c r="P7" s="11" t="s">
@@ -2190,27 +2191,27 @@
         <v>3</v>
       </c>
       <c r="V7" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>5.002174</v>
+      </c>
+      <c r="W7" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z7" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="13">
         <f t="shared" si="3"/>
-        <v>5.002174</v>
-      </c>
-      <c r="W7" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X7" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y7" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z7" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA7" s="13">
-        <f t="shared" si="7"/>
         <v>19958.669999999998</v>
       </c>
       <c r="AB7" s="13">
@@ -2218,7 +2219,7 @@
         <v>114999.98</v>
       </c>
       <c r="AC7" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>95041.31</v>
       </c>
       <c r="AD7" s="10" t="str">
@@ -2227,7 +2228,7 @@
       </c>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AG7" s="15" t="str">
@@ -2235,15 +2236,15 @@
         <v>33610006189-2</v>
       </c>
       <c r="AH7" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AI7" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK7" s="1">
@@ -2256,15 +2257,15 @@
         <v>114999.98</v>
       </c>
       <c r="AN7" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>95041.31</v>
       </c>
       <c r="AO7" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>5.0021740000000001</v>
       </c>
       <c r="AP7" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>115000</v>
       </c>
       <c r="AQ7" s="20">
@@ -2275,20 +2276,20 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B8" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C8" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D8" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B8" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
@@ -2313,7 +2314,7 @@
       </c>
       <c r="L8" s="1" t="str">
         <f t="shared" ref="L8:L13" ca="1" si="24">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Junio</v>
       </c>
       <c r="M8" s="4">
         <v>10.004348999999999</v>
@@ -2322,7 +2323,7 @@
         <v>19000</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>190082.63099999999</v>
       </c>
       <c r="P8" s="11" t="s">
@@ -2337,27 +2338,27 @@
         <v>2</v>
       </c>
       <c r="V8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>10.004349</v>
+      </c>
+      <c r="W8" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z8" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="13">
         <f t="shared" si="3"/>
-        <v>10.004349</v>
-      </c>
-      <c r="W8" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X8" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y8" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z8" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA8" s="13">
-        <f t="shared" si="7"/>
         <v>39917.35</v>
       </c>
       <c r="AB8" s="13">
@@ -2365,7 +2366,7 @@
         <v>229999.98</v>
       </c>
       <c r="AC8" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>190082.63</v>
       </c>
       <c r="AD8" s="10" t="str">
@@ -2374,7 +2375,7 @@
       </c>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="AG8" s="15" t="str">
@@ -2382,15 +2383,15 @@
         <v>33615420269-1</v>
       </c>
       <c r="AH8" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI8" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ8" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK8" s="1">
@@ -2403,15 +2404,15 @@
         <v>229999.98</v>
       </c>
       <c r="AN8" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>190082.63</v>
       </c>
       <c r="AO8" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AP8" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>230000</v>
       </c>
       <c r="AQ8" s="20">
@@ -2422,20 +2423,20 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B9" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C9" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D9" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B9" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -2460,7 +2461,7 @@
       </c>
       <c r="L9" s="1" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Junio</v>
       </c>
       <c r="M9" s="4">
         <v>1.0221830000000001</v>
@@ -2469,7 +2470,7 @@
         <v>19000</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>19421.477000000003</v>
       </c>
       <c r="P9" s="11" t="s">
@@ -2484,27 +2485,27 @@
         <v>2</v>
       </c>
       <c r="V9" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.022183</v>
+      </c>
+      <c r="W9" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z9" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="13">
         <f t="shared" si="3"/>
-        <v>1.022183</v>
-      </c>
-      <c r="W9" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X9" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y9" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z9" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA9" s="13">
-        <f t="shared" si="7"/>
         <v>4078.51</v>
       </c>
       <c r="AB9" s="13">
@@ -2512,7 +2513,7 @@
         <v>23499.99</v>
       </c>
       <c r="AC9" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>19421.48</v>
       </c>
       <c r="AD9" s="10" t="str">
@@ -2521,7 +2522,7 @@
       </c>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="AG9" s="15" t="str">
@@ -2529,15 +2530,15 @@
         <v>20147130202-1</v>
       </c>
       <c r="AH9" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI9" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ9" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK9" s="1">
@@ -2550,15 +2551,15 @@
         <v>23499.99</v>
       </c>
       <c r="AN9" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>19421.48</v>
       </c>
       <c r="AO9" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.0221830000000001</v>
       </c>
       <c r="AP9" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>23500</v>
       </c>
       <c r="AQ9" s="20">
@@ -2569,20 +2570,20 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B10" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C10" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D10" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B10" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -2607,7 +2608,7 @@
       </c>
       <c r="L10" s="1" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Junio</v>
       </c>
       <c r="M10" s="4">
         <v>1.0439320000000001</v>
@@ -2616,7 +2617,7 @@
         <v>19000</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>19834.708000000002</v>
       </c>
       <c r="P10" s="11" t="s">
@@ -2631,27 +2632,27 @@
         <v>2</v>
       </c>
       <c r="V10" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.043932</v>
+      </c>
+      <c r="W10" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z10" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="13">
         <f t="shared" si="3"/>
-        <v>1.043932</v>
-      </c>
-      <c r="W10" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X10" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y10" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z10" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA10" s="13">
-        <f t="shared" si="7"/>
         <v>4165.29</v>
       </c>
       <c r="AB10" s="13">
@@ -2659,7 +2660,7 @@
         <v>24000</v>
       </c>
       <c r="AC10" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>19834.71</v>
       </c>
       <c r="AD10" s="10" t="str">
@@ -2668,7 +2669,7 @@
       </c>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="AG10" s="15" t="str">
@@ -2676,15 +2677,15 @@
         <v>20374730429-1</v>
       </c>
       <c r="AH10" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI10" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ10" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK10" s="1">
@@ -2697,15 +2698,15 @@
         <v>24000</v>
       </c>
       <c r="AN10" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>19834.71</v>
       </c>
       <c r="AO10" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.0439320000000001</v>
       </c>
       <c r="AP10" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>24000</v>
       </c>
       <c r="AQ10" s="20">
@@ -2716,20 +2717,20 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B11" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C11" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D11" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B11" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -2754,7 +2755,7 @@
       </c>
       <c r="L11" s="1" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Junio</v>
       </c>
       <c r="M11" s="4">
         <v>1.3</v>
@@ -2763,7 +2764,7 @@
         <v>10000</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>13000</v>
       </c>
       <c r="P11" s="11" t="s">
@@ -2778,27 +2779,27 @@
         <v>2</v>
       </c>
       <c r="V11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="W11" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>10000.00</v>
+      </c>
+      <c r="X11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z11" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="13">
         <f t="shared" si="3"/>
-        <v>1.3</v>
-      </c>
-      <c r="W11" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>10000.00</v>
-      </c>
-      <c r="X11" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y11" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z11" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA11" s="13">
-        <f t="shared" si="7"/>
         <v>2256.1999999999998</v>
       </c>
       <c r="AB11" s="13">
@@ -2806,7 +2807,7 @@
         <v>13000</v>
       </c>
       <c r="AC11" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>13000.00</v>
       </c>
       <c r="AD11" s="10" t="str">
@@ -2815,7 +2816,7 @@
       </c>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="AG11" s="15" t="str">
@@ -2823,15 +2824,15 @@
         <v>37473042-1</v>
       </c>
       <c r="AH11" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AI11" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>B</v>
       </c>
       <c r="AK11" s="1">
@@ -2844,15 +2845,15 @@
         <v>13000</v>
       </c>
       <c r="AN11" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>10743.8</v>
       </c>
       <c r="AO11" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.3</v>
       </c>
       <c r="AP11" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>13000</v>
       </c>
       <c r="AQ11" s="20">
@@ -2863,20 +2864,20 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B12" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C12" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D12" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B12" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -2901,7 +2902,7 @@
       </c>
       <c r="L12" s="1" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Junio</v>
       </c>
       <c r="M12" s="4">
         <v>1.2105263157894737</v>
@@ -2910,7 +2911,7 @@
         <v>19000</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>23000</v>
       </c>
       <c r="P12" s="11" t="s">
@@ -2925,27 +2926,27 @@
         <v>2</v>
       </c>
       <c r="V12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.210526</v>
+      </c>
+      <c r="W12" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z12" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="13">
         <f t="shared" si="3"/>
-        <v>1.210526</v>
-      </c>
-      <c r="W12" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X12" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y12" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z12" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA12" s="13">
-        <f t="shared" si="7"/>
         <v>3991.74</v>
       </c>
       <c r="AB12" s="13">
@@ -2953,7 +2954,7 @@
         <v>23000</v>
       </c>
       <c r="AC12" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>23000.00</v>
       </c>
       <c r="AD12" s="10" t="str">
@@ -2962,7 +2963,7 @@
       </c>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="AG12" s="15" t="str">
@@ -2970,15 +2971,15 @@
         <v>30707354719-1</v>
       </c>
       <c r="AH12" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI12" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>B</v>
       </c>
       <c r="AK12" s="1">
@@ -2991,15 +2992,15 @@
         <v>23000</v>
       </c>
       <c r="AN12" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>19008.259999999998</v>
       </c>
       <c r="AO12" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.2105263157894737</v>
       </c>
       <c r="AP12" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>23000</v>
       </c>
       <c r="AQ12" s="20">
@@ -3010,20 +3011,20 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B13" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C13" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D13" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B13" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -3046,7 +3047,7 @@
       </c>
       <c r="L13" s="1" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Junio</v>
       </c>
       <c r="M13" s="4">
         <v>1.5</v>
@@ -3055,7 +3056,7 @@
         <v>19000</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>28500</v>
       </c>
       <c r="P13" s="11"/>
@@ -3068,27 +3069,27 @@
         <v>2</v>
       </c>
       <c r="V13" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="W13" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z13" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="13">
         <f t="shared" si="3"/>
-        <v>1.5</v>
-      </c>
-      <c r="W13" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X13" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y13" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z13" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA13" s="13">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB13" s="13">
@@ -3096,7 +3097,7 @@
         <v>28500</v>
       </c>
       <c r="AC13" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>28500.00</v>
       </c>
       <c r="AD13" s="10" t="str">
@@ -3105,7 +3106,7 @@
       </c>
       <c r="AE13" s="1"/>
       <c r="AF13" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="AG13" s="15" t="str">
@@ -3113,15 +3114,15 @@
         <v>-0</v>
       </c>
       <c r="AH13" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI13" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ13" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>C</v>
       </c>
       <c r="AK13" s="1">
@@ -3134,15 +3135,15 @@
         <v>28500</v>
       </c>
       <c r="AN13" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>28500</v>
       </c>
       <c r="AO13" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="AP13" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>28500</v>
       </c>
       <c r="AQ13" s="20">
@@ -3153,20 +3154,20 @@
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B14" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C14" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D14" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B14" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
@@ -3199,7 +3200,7 @@
         <v>19000</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>133471.06700000001</v>
       </c>
       <c r="P14" s="11" t="s">
@@ -3222,27 +3223,27 @@
         <v>2</v>
       </c>
       <c r="V14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>7.024793</v>
+      </c>
+      <c r="W14" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000150</v>
+      </c>
+      <c r="Z14" s="9">
+        <f t="shared" si="18"/>
+        <v>44816</v>
+      </c>
+      <c r="AA14" s="13">
         <f t="shared" si="3"/>
-        <v>7.024793</v>
-      </c>
-      <c r="W14" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X14" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00002</v>
-      </c>
-      <c r="Y14" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000150</v>
-      </c>
-      <c r="Z14" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="AA14" s="13">
-        <f t="shared" si="7"/>
         <v>28028.92</v>
       </c>
       <c r="AB14" s="13">
@@ -3250,7 +3251,7 @@
         <v>161499.99</v>
       </c>
       <c r="AC14" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>133471.07</v>
       </c>
       <c r="AD14" s="10" t="str">
@@ -3259,7 +3260,7 @@
       </c>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="AG14" s="15" t="str">
@@ -3267,15 +3268,15 @@
         <v>30684125792-1</v>
       </c>
       <c r="AH14" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK14" s="1">
@@ -3288,15 +3289,15 @@
         <v>161499.99</v>
       </c>
       <c r="AN14" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>133471.07</v>
       </c>
       <c r="AO14" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>7.0247929999999998</v>
       </c>
       <c r="AP14" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>161500</v>
       </c>
       <c r="AQ14" s="20">
@@ -3307,20 +3308,20 @@
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B15" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C15" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D15" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B15" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -3353,7 +3354,7 @@
         <v>19000</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>28500</v>
       </c>
       <c r="P15" s="11" t="s">
@@ -3376,27 +3377,27 @@
         <v>2</v>
       </c>
       <c r="V15" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="W15" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000152</v>
+      </c>
+      <c r="Z15" s="9">
+        <f t="shared" si="18"/>
+        <v>44816</v>
+      </c>
+      <c r="AA15" s="13">
         <f t="shared" si="3"/>
-        <v>1.5</v>
-      </c>
-      <c r="W15" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X15" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00002</v>
-      </c>
-      <c r="Y15" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000152</v>
-      </c>
-      <c r="Z15" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="AA15" s="13">
-        <f t="shared" si="7"/>
         <v>4946.28</v>
       </c>
       <c r="AB15" s="13">
@@ -3404,7 +3405,7 @@
         <v>28500</v>
       </c>
       <c r="AC15" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>28500.00</v>
       </c>
       <c r="AD15" s="10" t="str">
@@ -3413,7 +3414,7 @@
       </c>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="AG15" s="15" t="str">
@@ -3421,15 +3422,15 @@
         <v>30707354719-2</v>
       </c>
       <c r="AH15" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI15" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>B</v>
       </c>
       <c r="AK15" s="1">
@@ -3442,15 +3443,15 @@
         <v>28500</v>
       </c>
       <c r="AN15" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>23553.72</v>
       </c>
       <c r="AO15" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="AP15" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>28500</v>
       </c>
       <c r="AQ15" s="20">
@@ -3461,20 +3462,20 @@
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B16" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C16" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D16" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B16" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -3507,7 +3508,7 @@
         <v>19000</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>133057.83600000001</v>
       </c>
       <c r="P16" s="11" t="s">
@@ -3530,27 +3531,27 @@
         <v>2</v>
       </c>
       <c r="V16" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>7.003044</v>
+      </c>
+      <c r="W16" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000151</v>
+      </c>
+      <c r="Z16" s="9">
+        <f t="shared" si="18"/>
+        <v>44816</v>
+      </c>
+      <c r="AA16" s="13">
         <f t="shared" si="3"/>
-        <v>7.003044</v>
-      </c>
-      <c r="W16" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X16" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00002</v>
-      </c>
-      <c r="Y16" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000151</v>
-      </c>
-      <c r="Z16" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="AA16" s="13">
-        <f t="shared" si="7"/>
         <v>27942.15</v>
       </c>
       <c r="AB16" s="13">
@@ -3558,7 +3559,7 @@
         <v>160999.99</v>
       </c>
       <c r="AC16" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>133057.84</v>
       </c>
       <c r="AD16" s="10" t="str">
@@ -3567,7 +3568,7 @@
       </c>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="AG16" s="15" t="str">
@@ -3575,15 +3576,15 @@
         <v>30684125792-2</v>
       </c>
       <c r="AH16" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI16" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ16" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK16" s="1">
@@ -3596,15 +3597,15 @@
         <v>160999.98000000001</v>
       </c>
       <c r="AN16" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>133057.82999999999</v>
       </c>
       <c r="AO16" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>7.003044</v>
       </c>
       <c r="AP16" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>161000</v>
       </c>
       <c r="AQ16" s="20">
@@ -3615,20 +3616,20 @@
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B17" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C17" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D17" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45108</v>
+      </c>
+      <c r="B17" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45078</v>
+      </c>
+      <c r="C17" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45107</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45122</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -3661,7 +3662,7 @@
         <v>19000</v>
       </c>
       <c r="O17" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>28500</v>
       </c>
       <c r="P17" s="11" t="s">
@@ -3684,27 +3685,27 @@
         <v>2</v>
       </c>
       <c r="V17" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="W17" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000153</v>
+      </c>
+      <c r="Z17" s="9">
+        <f t="shared" si="18"/>
+        <v>44816</v>
+      </c>
+      <c r="AA17" s="13">
         <f t="shared" si="3"/>
-        <v>1.5</v>
-      </c>
-      <c r="W17" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X17" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00002</v>
-      </c>
-      <c r="Y17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000153</v>
-      </c>
-      <c r="Z17" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="AA17" s="13">
-        <f t="shared" si="7"/>
         <v>4946.28</v>
       </c>
       <c r="AB17" s="13">
@@ -3712,7 +3713,7 @@
         <v>28500</v>
       </c>
       <c r="AC17" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>28500.00</v>
       </c>
       <c r="AD17" s="10" t="str">
@@ -3721,7 +3722,7 @@
       </c>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="AG17" s="15" t="str">
@@ -3729,15 +3730,15 @@
         <v>37473042-2</v>
       </c>
       <c r="AH17" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI17" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>B</v>
       </c>
       <c r="AK17" s="1">
@@ -3750,15 +3751,15 @@
         <v>28500</v>
       </c>
       <c r="AN17" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>23553.72</v>
       </c>
       <c r="AO17" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="AP17" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>28500</v>
       </c>
       <c r="AQ17" s="20">

</xml_diff>

<commit_message>
Update Excel to add cod and bonif
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Facturador-Multiusuario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD680BF-2722-4D9A-9832-AD34BA28294E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F54E1BB-2FE6-400B-98BA-4EAA00B97F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Factura" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AP$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AU$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="88">
   <si>
     <t>Fecha</t>
   </si>
@@ -285,6 +285,21 @@
   </si>
   <si>
     <t>AUX unidades mult</t>
+  </si>
+  <si>
+    <t>Cod</t>
+  </si>
+  <si>
+    <t>Bonif</t>
+  </si>
+  <si>
+    <t>% Bonif</t>
+  </si>
+  <si>
+    <t>% Bonif (Facturador)</t>
+  </si>
+  <si>
+    <t>Bonif Facturador</t>
   </si>
 </sst>
 </file>
@@ -825,7 +840,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -849,6 +864,7 @@
     <xf numFmtId="2" fontId="0" fillId="35" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1211,12 +1227,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR17"/>
+  <dimension ref="A1:AW17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,29 +1246,32 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
     <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="25" width="9.140625" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" customWidth="1"/>
-    <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11" customWidth="1"/>
-    <col min="30" max="30" width="11.5703125" customWidth="1"/>
-    <col min="31" max="31" width="9.140625" customWidth="1"/>
-    <col min="32" max="32" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6" customWidth="1"/>
-    <col min="35" max="35" width="5.85546875" customWidth="1"/>
-    <col min="36" max="36" width="4" customWidth="1"/>
-    <col min="37" max="37" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="21" width="9.140625" customWidth="1"/>
+    <col min="22" max="25" width="8" customWidth="1"/>
+    <col min="26" max="30" width="9.140625" customWidth="1"/>
+    <col min="31" max="31" width="11" customWidth="1"/>
+    <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="9.140625" customWidth="1"/>
+    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6" customWidth="1"/>
+    <col min="40" max="40" width="5.85546875" customWidth="1"/>
+    <col min="41" max="41" width="4" customWidth="1"/>
+    <col min="42" max="42" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1290,118 +1309,133 @@
         <v>11</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AG1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AH1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AI1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AK1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AL1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="16" t="s">
+      <c r="AM1" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="AI1" s="16" t="s">
+      <c r="AN1" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="AJ1" s="16" t="s">
+      <c r="AO1" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="AK1" s="16" t="s">
+      <c r="AP1" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="AL1" s="16" t="s">
+      <c r="AQ1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" s="17" t="s">
+      <c r="AR1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="17" t="s">
+      <c r="AS1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="17" t="s">
+      <c r="AT1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AP1" s="19" t="s">
+      <c r="AU1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="AQ1" s="19" t="s">
+      <c r="AV1" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="AR1" s="19" t="s">
+      <c r="AW1" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f ca="1">TODAY()</f>
-        <v>45108</v>
+        <v>45140</v>
       </c>
       <c r="B2" s="9">
         <f ca="1">DATE(YEAR(C2),MONTH(C2),1)</f>
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="C2" s="9">
         <f ca="1">EOMONTH(A2,-1)</f>
-        <v>45107</v>
+        <v>45138</v>
       </c>
       <c r="D2" s="9">
         <f ca="1">A2+14</f>
-        <v>45122</v>
+        <v>45154</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -1427,127 +1461,138 @@
       <c r="L2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="2"/>
+      <c r="N2" s="4">
         <v>7.003044</v>
       </c>
-      <c r="N2" s="5">
+      <c r="O2" s="5">
         <v>19000</v>
       </c>
-      <c r="O2" s="5">
-        <f>M2*N2</f>
+      <c r="P2" s="5">
+        <f>N2*O2</f>
         <v>133057.83600000001</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="14">
+      <c r="T2" s="11"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="1" t="str">
+        <f>SUBSTITUTE(V2,",",".")</f>
+        <v/>
+      </c>
+      <c r="Y2" s="1" t="str">
+        <f t="shared" ref="Y2:Y17" si="0">SUBSTITUTE(W2,",",".")</f>
+        <v/>
+      </c>
+      <c r="Z2" s="14">
         <f>COUNTIFS($F$1:F2,F2,$K$1:K2,K2)+1</f>
         <v>2</v>
       </c>
-      <c r="V2" s="18" t="str">
-        <f t="shared" ref="V2:V17" si="0">SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
+      <c r="AA2" s="18" t="str">
+        <f t="shared" ref="AA2:AA17" si="1">SUBSTITUTE(IF(AO2="A",ROUND(P2/O2,6),ROUND(AG2/O2,6)),",",".")</f>
         <v>7.003044</v>
       </c>
-      <c r="W2" s="18" t="str">
-        <f>SUBSTITUTE(TEXT(N2,"0,00"),",",".")</f>
+      <c r="AB2" s="18" t="str">
+        <f>SUBSTITUTE(TEXT(O2,"0,00"),",",".")</f>
         <v>19000.00</v>
       </c>
-      <c r="X2" s="1" t="str">
-        <f t="shared" ref="X2:X17" si="1">TEXT(R2,"00000")</f>
+      <c r="AC2" s="1" t="str">
+        <f t="shared" ref="AC2:AC17" si="2">TEXT(S2,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="Y2" s="1" t="str">
-        <f t="shared" ref="Y2:Y17" si="2">TEXT(S2,"00000000")</f>
+      <c r="AD2" s="1" t="str">
+        <f t="shared" ref="AD2:AD17" si="3">TEXT(T2,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="Z2" s="9">
-        <f>T2</f>
-        <v>0</v>
-      </c>
-      <c r="AA2" s="13">
-        <f t="shared" ref="AA2:AA17" si="3">IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
+      <c r="AE2" s="9">
+        <f>U2</f>
+        <v>0</v>
+      </c>
+      <c r="AF2" s="13">
+        <f t="shared" ref="AF2:AF17" si="4">IF(AO2="A",ROUND(P2*Q2,2),ROUND(P2*Q2/(1+Q2),2))</f>
         <v>27942.15</v>
       </c>
-      <c r="AB2" s="13">
-        <f>IF(AJ2="A",ROUND(O2+AA2,2),ROUND(O2,2))</f>
+      <c r="AG2" s="13">
+        <f>IF(AO2="A",ROUND(P2+AF2,2),ROUND(P2,2))</f>
         <v>160999.99</v>
       </c>
-      <c r="AC2" s="10" t="str">
-        <f t="shared" ref="AC2:AC17" si="4">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
+      <c r="AH2" s="10" t="str">
+        <f>IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(P2,"0,00"),",","."),SUBSTITUTE(TEXT(AG2,"0,00"),",","."))</f>
         <v>133057.84</v>
       </c>
-      <c r="AD2" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AB2,0)-AB2,"0,00"),",",".")</f>
+      <c r="AI2" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AG2,0)-AG2,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1">
-        <f t="shared" ref="AF2:AF17" si="5">ROW(K2)</f>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1">
+        <f>ROW(K2)</f>
         <v>2</v>
       </c>
-      <c r="AG2" s="15" t="str">
+      <c r="AL2" s="15" t="str">
         <f>J2&amp;"-"&amp;COUNTIF($J$1:J2,J2)</f>
         <v>30525390086-1</v>
       </c>
-      <c r="AH2" s="1">
-        <f t="shared" ref="AH2:AH17" si="6">IF(K1=K2,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AI2" s="1">
-        <f t="shared" ref="AI2:AI17" si="7">IF(K2=K3,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="1" t="str">
-        <f t="shared" ref="AJ2:AJ17" si="8">RIGHT(F2)</f>
+      <c r="AM2" s="1">
+        <f>IF(K1=K2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN2" s="1">
+        <f>IF(K2=K3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1" t="str">
+        <f>RIGHT(F2)</f>
         <v>A</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AP2" s="1">
         <f>IF(LEFT(F2,4)="Nota",0,1)</f>
         <v>1</v>
       </c>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="13">
-        <f>IF(RIGHT(F2,1)="A",ROUND(N2*M2*(1+P2),2),AB2)</f>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="13">
+        <f>IF(RIGHT(F2,1)="A",ROUND(O2*N2*(1+Q2),2),AG2)</f>
         <v>160999.98000000001</v>
       </c>
-      <c r="AN2" s="13">
-        <f t="shared" ref="AN2:AN17" si="9">ROUND((AM2/(1+P2)),2)</f>
+      <c r="AS2" s="13">
+        <f t="shared" ref="AS2:AS17" si="5">ROUND((AR2/(1+Q2)),2)</f>
         <v>133057.82999999999</v>
       </c>
-      <c r="AO2" s="20">
-        <f t="shared" ref="AO2:AO17" si="10">IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
+      <c r="AT2" s="20">
+        <f t="shared" ref="AT2:AT17" si="6">IF(AO2="A",ROUND(AS2/O2,6),AR2/O2)</f>
         <v>7.003044</v>
       </c>
-      <c r="AP2" s="13">
-        <f t="shared" ref="AP2:AP17" si="11">IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
+      <c r="AU2" s="13">
+        <f t="shared" ref="AU2:AU17" si="7">IF(AO2="A",ROUND(CEILING(O2*N2*(1+Q2),500),2),ROUND(CEILING(O2*N2,500),2))</f>
         <v>161000</v>
       </c>
-      <c r="AQ2" s="20">
-        <f>IF(AJ2="A",ROUND(AN2/N2,6),AP2/N2)</f>
+      <c r="AV2" s="20">
+        <f>IF(AO2="A",ROUND(AS2/O2,6),AU2/O2)</f>
         <v>7.003044</v>
       </c>
-      <c r="AR2" s="2"/>
+      <c r="AW2" s="2"/>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f t="shared" ref="A3:A17" ca="1" si="12">TODAY()</f>
+        <f t="shared" ref="A3:A17" ca="1" si="8">TODAY()</f>
+        <v>45140</v>
+      </c>
+      <c r="B3" s="9">
+        <f t="shared" ref="B3:B17" ca="1" si="9">DATE(YEAR(C3),MONTH(C3),1)</f>
         <v>45108</v>
       </c>
-      <c r="B3" s="9">
-        <f t="shared" ref="B3:B17" ca="1" si="13">DATE(YEAR(C3),MONTH(C3),1)</f>
-        <v>45078</v>
-      </c>
       <c r="C3" s="9">
-        <f t="shared" ref="C3:C17" ca="1" si="14">EOMONTH(A3,-1)</f>
-        <v>45107</v>
+        <f t="shared" ref="C3:C17" ca="1" si="10">EOMONTH(A3,-1)</f>
+        <v>45138</v>
       </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:D17" ca="1" si="15">A3+14</f>
-        <v>45122</v>
+        <f t="shared" ref="D3:D17" ca="1" si="11">A3+14</f>
+        <v>45154</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1572,129 +1617,140 @@
       </c>
       <c r="L3" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B3,"mmmm"))</f>
-        <v>Honorarios Junio</v>
-      </c>
-      <c r="M3" s="4">
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="4">
         <v>8.0252280000000003</v>
       </c>
-      <c r="N3" s="5">
+      <c r="O3" s="5">
         <v>19000</v>
       </c>
-      <c r="O3" s="5">
-        <f t="shared" ref="O3:O17" si="16">M3*N3</f>
+      <c r="P3" s="5">
+        <f t="shared" ref="P3:P17" si="12">N3*O3</f>
         <v>152479.33199999999</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="14">
+      <c r="T3" s="11"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="1" t="str">
+        <f t="shared" ref="X3:X17" si="13">SUBSTITUTE(V3,",",".")</f>
+        <v/>
+      </c>
+      <c r="Y3" s="1" t="str">
+        <f>SUBSTITUTE(W3,",",".")</f>
+        <v/>
+      </c>
+      <c r="Z3" s="14">
         <f>COUNTIFS($F$1:F3,F3,$K$1:K3,K3)+1</f>
         <v>2</v>
       </c>
-      <c r="V3" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA3" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>8.025228</v>
       </c>
-      <c r="W3" s="18" t="str">
-        <f t="shared" ref="W3:W17" si="17">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
+      <c r="AB3" s="18" t="str">
+        <f t="shared" ref="AB3:AB17" si="14">SUBSTITUTE(TEXT(O3,"0,00"),",",".")</f>
         <v>19000.00</v>
       </c>
-      <c r="X3" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC3" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y3" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD3" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z3" s="9">
-        <f t="shared" ref="Z3:Z17" si="18">T3</f>
-        <v>0</v>
-      </c>
-      <c r="AA3" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE3" s="9">
+        <f t="shared" ref="AE3:AE17" si="15">U3</f>
+        <v>0</v>
+      </c>
+      <c r="AF3" s="13">
+        <f t="shared" si="4"/>
         <v>32020.66</v>
       </c>
-      <c r="AB3" s="13">
-        <f t="shared" ref="AB3:AB17" si="19">IF(AJ3="A",ROUND(O3+AA3,2),ROUND(O3,2))</f>
+      <c r="AG3" s="13">
+        <f t="shared" ref="AG3:AG17" si="16">IF(AO3="A",ROUND(P3+AF3,2),ROUND(P3,2))</f>
         <v>184499.99</v>
       </c>
-      <c r="AC3" s="10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH3" s="10" t="str">
+        <f>IF(RIGHT(F3,1)="A",SUBSTITUTE(TEXT(P3,"0,00"),",","."),SUBSTITUTE(TEXT(AG3,"0,00"),",","."))</f>
         <v>152479.33</v>
       </c>
-      <c r="AD3" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AB3,0)-AB3,"0,00"),",",".")</f>
+      <c r="AI3" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AG3,0)-AG3,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1">
+        <f>ROW(K3)</f>
         <v>3</v>
       </c>
-      <c r="AG3" s="15" t="str">
+      <c r="AL3" s="15" t="str">
         <f>J3&amp;"-"&amp;COUNTIF($J$1:J3,J3)</f>
         <v>30525733870-1</v>
       </c>
-      <c r="AH3" s="1">
+      <c r="AM3" s="1">
+        <f>IF(K2=K3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN3" s="1">
+        <f>IF(K3=K4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO3" s="1" t="str">
+        <f>RIGHT(F3)</f>
+        <v>A</v>
+      </c>
+      <c r="AP3" s="1">
+        <f>IF(LEFT(F3,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="13">
+        <f>IF(RIGHT(F3,1)="A",ROUND(O3*N3*(1+Q3),2),AG3)</f>
+        <v>184499.99</v>
+      </c>
+      <c r="AS3" s="13">
+        <f t="shared" si="5"/>
+        <v>152479.32999999999</v>
+      </c>
+      <c r="AT3" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI3" s="1">
+        <v>8.0252280000000003</v>
+      </c>
+      <c r="AU3" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK3" s="1">
-        <f t="shared" ref="AK3:AK17" si="20">IF(LEFT(F3,4)="Nota",0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="13">
-        <f t="shared" ref="AM3:AM17" si="21">IF(RIGHT(F3,1)="A",ROUND(N3*M3*(1+P3),2),AB3)</f>
-        <v>184499.99</v>
-      </c>
-      <c r="AN3" s="13">
-        <f t="shared" si="9"/>
-        <v>152479.32999999999</v>
-      </c>
-      <c r="AO3" s="20">
-        <f t="shared" si="10"/>
+        <v>184500</v>
+      </c>
+      <c r="AV3" s="20">
+        <f t="shared" ref="AV3:AV17" si="17">IF(AO3="A",ROUND(AS3/O3,6),AU3/O3)</f>
         <v>8.0252280000000003</v>
       </c>
-      <c r="AP3" s="13">
-        <f t="shared" si="11"/>
-        <v>184500</v>
-      </c>
-      <c r="AQ3" s="20">
-        <f t="shared" ref="AQ3:AQ17" si="22">IF(AJ3="A",ROUND(AN3/N3,6),AP3/N3)</f>
-        <v>8.0252280000000003</v>
-      </c>
-      <c r="AR3" s="2"/>
+      <c r="AW3" s="2"/>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B4" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B4" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C4" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1719,129 +1775,140 @@
       </c>
       <c r="L4" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
-        <v>Honorarios Junio</v>
-      </c>
-      <c r="M4" s="4">
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="4">
         <v>10.004348999999999</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="5">
         <v>19000</v>
       </c>
-      <c r="O4" s="5">
-        <f t="shared" si="16"/>
+      <c r="P4" s="5">
+        <f t="shared" si="12"/>
         <v>190082.63099999999</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="14">
+      <c r="T4" s="11"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <f t="shared" ref="Y4:Y17" si="18">SUBSTITUTE(W4,",",".")</f>
+        <v/>
+      </c>
+      <c r="Z4" s="14">
         <f>COUNTIFS($F$1:F4,F4,$K$1:K4,K4)+1</f>
         <v>2</v>
       </c>
-      <c r="V4" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA4" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>10.004349</v>
       </c>
-      <c r="W4" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB4" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X4" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC4" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y4" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD4" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z4" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA4" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE4" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="13">
+        <f t="shared" si="4"/>
         <v>39917.35</v>
       </c>
-      <c r="AB4" s="13">
-        <f t="shared" si="19"/>
+      <c r="AG4" s="13">
+        <f t="shared" si="16"/>
         <v>229999.98</v>
       </c>
-      <c r="AC4" s="10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH4" s="10" t="str">
+        <f>IF(RIGHT(F4,1)="A",SUBSTITUTE(TEXT(P4,"0,00"),",","."),SUBSTITUTE(TEXT(AG4,"0,00"),",","."))</f>
         <v>190082.63</v>
       </c>
-      <c r="AD4" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AB4,0)-AB4,"0,00"),",",".")</f>
+      <c r="AI4" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AG4,0)-AG4,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1">
+        <f>ROW(K4)</f>
         <v>4</v>
       </c>
-      <c r="AG4" s="15" t="str">
+      <c r="AL4" s="15" t="str">
         <f>J4&amp;"-"&amp;COUNTIF($J$1:J4,J4)</f>
         <v>30610252334-1</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AM4" s="1">
+        <f>IF(K3=K4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN4" s="1">
+        <f>IF(K4=K5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO4" s="1" t="str">
+        <f>RIGHT(F4)</f>
+        <v>A</v>
+      </c>
+      <c r="AP4" s="1">
+        <f>IF(LEFT(F4,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="13">
+        <f>IF(RIGHT(F4,1)="A",ROUND(O4*N4*(1+Q4),2),AG4)</f>
+        <v>229999.98</v>
+      </c>
+      <c r="AS4" s="13">
+        <f t="shared" si="5"/>
+        <v>190082.63</v>
+      </c>
+      <c r="AT4" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI4" s="1">
+        <v>10.004348999999999</v>
+      </c>
+      <c r="AU4" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK4" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL4" s="2"/>
-      <c r="AM4" s="13">
-        <f t="shared" si="21"/>
-        <v>229999.98</v>
-      </c>
-      <c r="AN4" s="13">
-        <f t="shared" si="9"/>
-        <v>190082.63</v>
-      </c>
-      <c r="AO4" s="20">
-        <f t="shared" si="10"/>
+        <v>230000</v>
+      </c>
+      <c r="AV4" s="20">
+        <f t="shared" si="17"/>
         <v>10.004348999999999</v>
       </c>
-      <c r="AP4" s="13">
-        <f t="shared" si="11"/>
-        <v>230000</v>
-      </c>
-      <c r="AQ4" s="20">
-        <f t="shared" si="22"/>
-        <v>10.004348999999999</v>
-      </c>
-      <c r="AR4" s="2"/>
+      <c r="AW4" s="2"/>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B5" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B5" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C5" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D5" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -1866,129 +1933,140 @@
       </c>
       <c r="L5" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B5,"mmmm"))</f>
-        <v>Honorarios Junio</v>
-      </c>
-      <c r="M5" s="4">
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="4">
         <v>9.0256629999999998</v>
       </c>
-      <c r="N5" s="5">
+      <c r="O5" s="5">
         <v>19000</v>
       </c>
-      <c r="O5" s="5">
-        <f t="shared" si="16"/>
+      <c r="P5" s="5">
+        <f t="shared" si="12"/>
         <v>171487.59700000001</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
       <c r="S5" s="11"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="14">
+      <c r="T5" s="11"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y5" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z5" s="14">
         <f>COUNTIFS($F$1:F5,F5,$K$1:K5,K5)+1</f>
         <v>2</v>
       </c>
-      <c r="V5" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA5" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>9.025663</v>
       </c>
-      <c r="W5" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB5" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X5" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC5" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y5" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD5" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z5" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE5" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="13">
+        <f t="shared" si="4"/>
         <v>36012.400000000001</v>
       </c>
-      <c r="AB5" s="13">
-        <f t="shared" si="19"/>
+      <c r="AG5" s="13">
+        <f t="shared" si="16"/>
         <v>207500</v>
       </c>
-      <c r="AC5" s="10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH5" s="10" t="str">
+        <f>IF(RIGHT(F5,1)="A",SUBSTITUTE(TEXT(P5,"0,00"),",","."),SUBSTITUTE(TEXT(AG5,"0,00"),",","."))</f>
         <v>171487.60</v>
       </c>
-      <c r="AD5" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AB5,0)-AB5,"0,00"),",",".")</f>
+      <c r="AI5" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AG5,0)-AG5,"0,00"),",",".")</f>
         <v>0.00</v>
       </c>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1">
+        <f>ROW(K5)</f>
         <v>5</v>
       </c>
-      <c r="AG5" s="15" t="str">
+      <c r="AL5" s="15" t="str">
         <f>J5&amp;"-"&amp;COUNTIF($J$1:J5,J5)</f>
         <v>30710964277-1</v>
       </c>
-      <c r="AH5" s="1">
+      <c r="AM5" s="1">
+        <f>IF(K4=K5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN5" s="1">
+        <f>IF(K5=K6,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO5" s="1" t="str">
+        <f>RIGHT(F5)</f>
+        <v>A</v>
+      </c>
+      <c r="AP5" s="1">
+        <f>IF(LEFT(F5,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="13">
+        <f>IF(RIGHT(F5,1)="A",ROUND(O5*N5*(1+Q5),2),AG5)</f>
+        <v>207499.99</v>
+      </c>
+      <c r="AS5" s="13">
+        <f t="shared" si="5"/>
+        <v>171487.6</v>
+      </c>
+      <c r="AT5" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI5" s="1">
+        <v>9.0256629999999998</v>
+      </c>
+      <c r="AU5" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK5" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL5" s="2"/>
-      <c r="AM5" s="13">
-        <f t="shared" si="21"/>
-        <v>207499.99</v>
-      </c>
-      <c r="AN5" s="13">
-        <f t="shared" si="9"/>
-        <v>171487.6</v>
-      </c>
-      <c r="AO5" s="20">
-        <f t="shared" si="10"/>
+        <v>207500</v>
+      </c>
+      <c r="AV5" s="20">
+        <f t="shared" si="17"/>
         <v>9.0256629999999998</v>
       </c>
-      <c r="AP5" s="13">
-        <f t="shared" si="11"/>
-        <v>207500</v>
-      </c>
-      <c r="AQ5" s="20">
-        <f t="shared" si="22"/>
-        <v>9.0256629999999998</v>
-      </c>
-      <c r="AR5" s="2"/>
+      <c r="AW5" s="2"/>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B6" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B6" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C6" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D6" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -2013,137 +2091,148 @@
       </c>
       <c r="L6" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B6,"mmmm"))</f>
-        <v>Honorarios Junio</v>
-      </c>
-      <c r="M6" s="4">
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="4">
         <v>5.0239229999999999</v>
       </c>
-      <c r="N6" s="5">
+      <c r="O6" s="5">
         <v>19000</v>
       </c>
-      <c r="O6" s="5">
-        <f t="shared" si="16"/>
+      <c r="P6" s="5">
+        <f t="shared" si="12"/>
         <v>95454.536999999997</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="Q6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="R6" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="S6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="T6" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="T6" s="12">
+      <c r="U6" s="12">
         <v>44816</v>
       </c>
-      <c r="U6" s="14">
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y6" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z6" s="14">
         <f>COUNTIFS($F$1:F6,F6,$K$1:K6,K6)+1</f>
         <v>2</v>
       </c>
-      <c r="V6" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA6" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>5.023923</v>
       </c>
-      <c r="W6" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB6" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X6" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC6" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00002</v>
       </c>
-      <c r="Y6" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD6" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000003</v>
       </c>
-      <c r="Z6" s="9">
-        <f t="shared" si="18"/>
+      <c r="AE6" s="9">
+        <f t="shared" si="15"/>
         <v>44816</v>
       </c>
-      <c r="AA6" s="13">
-        <f t="shared" si="3"/>
+      <c r="AF6" s="13">
+        <f t="shared" si="4"/>
         <v>20045.45</v>
       </c>
-      <c r="AB6" s="13">
-        <f t="shared" si="19"/>
+      <c r="AG6" s="13">
+        <f t="shared" si="16"/>
         <v>115499.99</v>
       </c>
-      <c r="AC6" s="10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH6" s="10" t="str">
+        <f>IF(RIGHT(F6,1)="A",SUBSTITUTE(TEXT(P6,"0,00"),",","."),SUBSTITUTE(TEXT(AG6,"0,00"),",","."))</f>
         <v>95454.54</v>
       </c>
-      <c r="AD6" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AB6,0)-AB6,"0,00"),",",".")</f>
+      <c r="AI6" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AG6,0)-AG6,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1">
+        <f>ROW(K6)</f>
         <v>6</v>
       </c>
-      <c r="AG6" s="15" t="str">
+      <c r="AL6" s="15" t="str">
         <f>J6&amp;"-"&amp;COUNTIF($J$1:J6,J6)</f>
         <v>33610006189-1</v>
       </c>
-      <c r="AH6" s="1">
+      <c r="AM6" s="1">
+        <f>IF(K5=K6,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN6" s="1">
+        <f>IF(K6=K7,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO6" s="1" t="str">
+        <f>RIGHT(F6)</f>
+        <v>A</v>
+      </c>
+      <c r="AP6" s="1">
+        <f>IF(LEFT(F6,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="13">
+        <f>IF(RIGHT(F6,1)="A",ROUND(O6*N6*(1+Q6),2),AG6)</f>
+        <v>115499.99</v>
+      </c>
+      <c r="AS6" s="13">
+        <f t="shared" si="5"/>
+        <v>95454.54</v>
+      </c>
+      <c r="AT6" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI6" s="1">
+        <v>5.0239229999999999</v>
+      </c>
+      <c r="AU6" s="13">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK6" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL6" s="2"/>
-      <c r="AM6" s="13">
-        <f t="shared" si="21"/>
-        <v>115499.99</v>
-      </c>
-      <c r="AN6" s="13">
-        <f t="shared" si="9"/>
-        <v>95454.54</v>
-      </c>
-      <c r="AO6" s="20">
-        <f t="shared" si="10"/>
+        <v>115500</v>
+      </c>
+      <c r="AV6" s="20">
+        <f t="shared" si="17"/>
         <v>5.0239229999999999</v>
       </c>
-      <c r="AP6" s="13">
-        <f t="shared" si="11"/>
-        <v>115500</v>
-      </c>
-      <c r="AQ6" s="20">
-        <f t="shared" si="22"/>
-        <v>5.0239229999999999</v>
-      </c>
-      <c r="AR6" s="2"/>
+      <c r="AW6" s="2"/>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B7" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B7" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C7" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D7" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2169,127 +2258,138 @@
       <c r="L7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="2"/>
+      <c r="N7" s="4">
         <v>5.0021740000000001</v>
       </c>
-      <c r="N7" s="5">
+      <c r="O7" s="5">
         <v>19000</v>
       </c>
-      <c r="O7" s="5">
-        <f t="shared" si="16"/>
+      <c r="P7" s="5">
+        <f t="shared" si="12"/>
         <v>95041.305999999997</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="Q7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="14">
+      <c r="T7" s="11"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y7" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z7" s="14">
         <f>COUNTIFS($F$1:F7,F7,$K$1:K7,K7)+1</f>
         <v>3</v>
       </c>
-      <c r="V7" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA7" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>5.002174</v>
       </c>
-      <c r="W7" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB7" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X7" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC7" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y7" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD7" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z7" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA7" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE7" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="13">
+        <f t="shared" si="4"/>
         <v>19958.669999999998</v>
       </c>
-      <c r="AB7" s="13">
-        <f t="shared" si="19"/>
+      <c r="AG7" s="13">
+        <f t="shared" si="16"/>
         <v>114999.98</v>
       </c>
-      <c r="AC7" s="10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH7" s="10" t="str">
+        <f>IF(RIGHT(F7,1)="A",SUBSTITUTE(TEXT(P7,"0,00"),",","."),SUBSTITUTE(TEXT(AG7,"0,00"),",","."))</f>
         <v>95041.31</v>
       </c>
-      <c r="AD7" s="10" t="str">
-        <f t="shared" ref="AD7:AD17" si="23">SUBSTITUTE(TEXT(ROUNDUP(AB7,0)-AB7,"0,00"),",",".")</f>
+      <c r="AI7" s="10" t="str">
+        <f t="shared" ref="AI7:AI17" si="19">SUBSTITUTE(TEXT(ROUNDUP(AG7,0)-AG7,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1">
+        <f>ROW(K7)</f>
         <v>7</v>
       </c>
-      <c r="AG7" s="15" t="str">
+      <c r="AL7" s="15" t="str">
         <f>J7&amp;"-"&amp;COUNTIF($J$1:J7,J7)</f>
         <v>33610006189-2</v>
       </c>
-      <c r="AH7" s="1">
+      <c r="AM7" s="1">
+        <f>IF(K6=K7,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AN7" s="1">
+        <f>IF(K7=K8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO7" s="1" t="str">
+        <f>RIGHT(F7)</f>
+        <v>A</v>
+      </c>
+      <c r="AP7" s="1">
+        <f>IF(LEFT(F7,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="13">
+        <f>IF(RIGHT(F7,1)="A",ROUND(O7*N7*(1+Q7),2),AG7)</f>
+        <v>114999.98</v>
+      </c>
+      <c r="AS7" s="13">
+        <f t="shared" si="5"/>
+        <v>95041.31</v>
+      </c>
+      <c r="AT7" s="20">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AI7" s="1">
+        <v>5.0021740000000001</v>
+      </c>
+      <c r="AU7" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK7" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL7" s="2"/>
-      <c r="AM7" s="13">
-        <f t="shared" si="21"/>
-        <v>114999.98</v>
-      </c>
-      <c r="AN7" s="13">
-        <f t="shared" si="9"/>
-        <v>95041.31</v>
-      </c>
-      <c r="AO7" s="20">
-        <f t="shared" si="10"/>
+        <v>115000</v>
+      </c>
+      <c r="AV7" s="20">
+        <f t="shared" si="17"/>
         <v>5.0021740000000001</v>
       </c>
-      <c r="AP7" s="13">
-        <f t="shared" si="11"/>
-        <v>115000</v>
-      </c>
-      <c r="AQ7" s="20">
-        <f t="shared" si="22"/>
-        <v>5.0021740000000001</v>
-      </c>
-      <c r="AR7" s="2"/>
+      <c r="AW7" s="2"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B8" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B8" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C8" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D8" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
@@ -2313,130 +2413,141 @@
         <v>52</v>
       </c>
       <c r="L8" s="1" t="str">
-        <f t="shared" ref="L8:L13" ca="1" si="24">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
-        <v>Honorarios Junio</v>
-      </c>
-      <c r="M8" s="4">
+        <f t="shared" ref="L8:L13" ca="1" si="20">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="4">
         <v>10.004348999999999</v>
       </c>
-      <c r="N8" s="5">
+      <c r="O8" s="5">
         <v>19000</v>
       </c>
-      <c r="O8" s="5">
-        <f t="shared" si="16"/>
+      <c r="P8" s="5">
+        <f t="shared" si="12"/>
         <v>190082.63099999999</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="14">
+      <c r="T8" s="11"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y8" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z8" s="14">
         <f>COUNTIFS($F$1:F8,F8,$K$1:K8,K8)+1</f>
         <v>2</v>
       </c>
-      <c r="V8" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA8" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>10.004349</v>
       </c>
-      <c r="W8" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB8" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X8" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC8" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y8" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD8" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z8" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE8" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="13">
+        <f t="shared" si="4"/>
         <v>39917.35</v>
       </c>
-      <c r="AB8" s="13">
+      <c r="AG8" s="13">
+        <f t="shared" si="16"/>
+        <v>229999.98</v>
+      </c>
+      <c r="AH8" s="10" t="str">
+        <f>IF(RIGHT(F8,1)="A",SUBSTITUTE(TEXT(P8,"0,00"),",","."),SUBSTITUTE(TEXT(AG8,"0,00"),",","."))</f>
+        <v>190082.63</v>
+      </c>
+      <c r="AI8" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>229999.98</v>
-      </c>
-      <c r="AC8" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>190082.63</v>
-      </c>
-      <c r="AD8" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.02</v>
       </c>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1">
+        <f>ROW(K8)</f>
         <v>8</v>
       </c>
-      <c r="AG8" s="15" t="str">
+      <c r="AL8" s="15" t="str">
         <f>J8&amp;"-"&amp;COUNTIF($J$1:J8,J8)</f>
         <v>33615420269-1</v>
       </c>
-      <c r="AH8" s="1">
+      <c r="AM8" s="1">
+        <f>IF(K7=K8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN8" s="1">
+        <f>IF(K8=K9,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO8" s="1" t="str">
+        <f>RIGHT(F8)</f>
+        <v>A</v>
+      </c>
+      <c r="AP8" s="1">
+        <f>IF(LEFT(F8,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="13">
+        <f>IF(RIGHT(F8,1)="A",ROUND(O8*N8*(1+Q8),2),AG8)</f>
+        <v>229999.98</v>
+      </c>
+      <c r="AS8" s="13">
+        <f t="shared" si="5"/>
+        <v>190082.63</v>
+      </c>
+      <c r="AT8" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI8" s="1">
+        <v>10.004348999999999</v>
+      </c>
+      <c r="AU8" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK8" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL8" s="2"/>
-      <c r="AM8" s="13">
-        <f t="shared" si="21"/>
-        <v>229999.98</v>
-      </c>
-      <c r="AN8" s="13">
-        <f t="shared" si="9"/>
-        <v>190082.63</v>
-      </c>
-      <c r="AO8" s="20">
-        <f t="shared" si="10"/>
+        <v>230000</v>
+      </c>
+      <c r="AV8" s="20">
+        <f t="shared" si="17"/>
         <v>10.004348999999999</v>
       </c>
-      <c r="AP8" s="13">
-        <f t="shared" si="11"/>
-        <v>230000</v>
-      </c>
-      <c r="AQ8" s="20">
-        <f t="shared" si="22"/>
-        <v>10.004348999999999</v>
-      </c>
-      <c r="AR8" s="2"/>
+      <c r="AW8" s="2"/>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B9" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B9" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C9" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D9" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -2460,130 +2571,141 @@
         <v>57</v>
       </c>
       <c r="L9" s="1" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Junio</v>
-      </c>
-      <c r="M9" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="4">
         <v>1.0221830000000001</v>
       </c>
-      <c r="N9" s="5">
+      <c r="O9" s="5">
         <v>19000</v>
       </c>
-      <c r="O9" s="5">
-        <f t="shared" si="16"/>
+      <c r="P9" s="5">
+        <f t="shared" si="12"/>
         <v>19421.477000000003</v>
       </c>
-      <c r="P9" s="11" t="s">
+      <c r="Q9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="14">
+      <c r="T9" s="11"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y9" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z9" s="14">
         <f>COUNTIFS($F$1:F9,F9,$K$1:K9,K9)+1</f>
         <v>2</v>
       </c>
-      <c r="V9" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA9" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>1.022183</v>
       </c>
-      <c r="W9" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB9" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X9" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC9" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y9" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD9" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z9" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE9" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF9" s="13">
+        <f t="shared" si="4"/>
         <v>4078.51</v>
       </c>
-      <c r="AB9" s="13">
+      <c r="AG9" s="13">
+        <f t="shared" si="16"/>
+        <v>23499.99</v>
+      </c>
+      <c r="AH9" s="10" t="str">
+        <f>IF(RIGHT(F9,1)="A",SUBSTITUTE(TEXT(P9,"0,00"),",","."),SUBSTITUTE(TEXT(AG9,"0,00"),",","."))</f>
+        <v>19421.48</v>
+      </c>
+      <c r="AI9" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>23499.99</v>
-      </c>
-      <c r="AC9" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>19421.48</v>
-      </c>
-      <c r="AD9" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1">
+        <f>ROW(K9)</f>
         <v>9</v>
       </c>
-      <c r="AG9" s="15" t="str">
+      <c r="AL9" s="15" t="str">
         <f>J9&amp;"-"&amp;COUNTIF($J$1:J9,J9)</f>
         <v>20147130202-1</v>
       </c>
-      <c r="AH9" s="1">
+      <c r="AM9" s="1">
+        <f>IF(K8=K9,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN9" s="1">
+        <f>IF(K9=K10,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO9" s="1" t="str">
+        <f>RIGHT(F9)</f>
+        <v>A</v>
+      </c>
+      <c r="AP9" s="1">
+        <f>IF(LEFT(F9,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="13">
+        <f>IF(RIGHT(F9,1)="A",ROUND(O9*N9*(1+Q9),2),AG9)</f>
+        <v>23499.99</v>
+      </c>
+      <c r="AS9" s="13">
+        <f t="shared" si="5"/>
+        <v>19421.48</v>
+      </c>
+      <c r="AT9" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI9" s="1">
+        <v>1.0221830000000001</v>
+      </c>
+      <c r="AU9" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK9" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL9" s="2"/>
-      <c r="AM9" s="13">
-        <f t="shared" si="21"/>
-        <v>23499.99</v>
-      </c>
-      <c r="AN9" s="13">
-        <f t="shared" si="9"/>
-        <v>19421.48</v>
-      </c>
-      <c r="AO9" s="20">
-        <f t="shared" si="10"/>
+        <v>23500</v>
+      </c>
+      <c r="AV9" s="20">
+        <f t="shared" si="17"/>
         <v>1.0221830000000001</v>
       </c>
-      <c r="AP9" s="13">
-        <f t="shared" si="11"/>
-        <v>23500</v>
-      </c>
-      <c r="AQ9" s="20">
-        <f t="shared" si="22"/>
-        <v>1.0221830000000001</v>
-      </c>
-      <c r="AR9" s="2"/>
+      <c r="AW9" s="2"/>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B10" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B10" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C10" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D10" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -2607,130 +2729,141 @@
         <v>56</v>
       </c>
       <c r="L10" s="1" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Junio</v>
-      </c>
-      <c r="M10" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="4">
         <v>1.0439320000000001</v>
       </c>
-      <c r="N10" s="5">
+      <c r="O10" s="5">
         <v>19000</v>
       </c>
-      <c r="O10" s="5">
-        <f t="shared" si="16"/>
+      <c r="P10" s="5">
+        <f t="shared" si="12"/>
         <v>19834.708000000002</v>
       </c>
-      <c r="P10" s="11" t="s">
+      <c r="Q10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="14">
+      <c r="T10" s="11"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y10" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z10" s="14">
         <f>COUNTIFS($F$1:F10,F10,$K$1:K10,K10)+1</f>
         <v>2</v>
       </c>
-      <c r="V10" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA10" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>1.043932</v>
       </c>
-      <c r="W10" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB10" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X10" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC10" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y10" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD10" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z10" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA10" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE10" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="13">
+        <f t="shared" si="4"/>
         <v>4165.29</v>
       </c>
-      <c r="AB10" s="13">
+      <c r="AG10" s="13">
+        <f t="shared" si="16"/>
+        <v>24000</v>
+      </c>
+      <c r="AH10" s="10" t="str">
+        <f>IF(RIGHT(F10,1)="A",SUBSTITUTE(TEXT(P10,"0,00"),",","."),SUBSTITUTE(TEXT(AG10,"0,00"),",","."))</f>
+        <v>19834.71</v>
+      </c>
+      <c r="AI10" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>24000</v>
-      </c>
-      <c r="AC10" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>19834.71</v>
-      </c>
-      <c r="AD10" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1">
+        <f>ROW(K10)</f>
         <v>10</v>
       </c>
-      <c r="AG10" s="15" t="str">
+      <c r="AL10" s="15" t="str">
         <f>J10&amp;"-"&amp;COUNTIF($J$1:J10,J10)</f>
         <v>20374730429-1</v>
       </c>
-      <c r="AH10" s="1">
+      <c r="AM10" s="1">
+        <f>IF(K9=K10,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN10" s="1">
+        <f>IF(K10=K11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO10" s="1" t="str">
+        <f>RIGHT(F10)</f>
+        <v>A</v>
+      </c>
+      <c r="AP10" s="1">
+        <f>IF(LEFT(F10,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="13">
+        <f>IF(RIGHT(F10,1)="A",ROUND(O10*N10*(1+Q10),2),AG10)</f>
+        <v>24000</v>
+      </c>
+      <c r="AS10" s="13">
+        <f t="shared" si="5"/>
+        <v>19834.71</v>
+      </c>
+      <c r="AT10" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI10" s="1">
+        <v>1.0439320000000001</v>
+      </c>
+      <c r="AU10" s="13">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AJ10" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK10" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL10" s="2"/>
-      <c r="AM10" s="13">
-        <f t="shared" si="21"/>
         <v>24000</v>
       </c>
-      <c r="AN10" s="13">
-        <f t="shared" si="9"/>
-        <v>19834.71</v>
-      </c>
-      <c r="AO10" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV10" s="20">
+        <f t="shared" si="17"/>
         <v>1.0439320000000001</v>
       </c>
-      <c r="AP10" s="13">
-        <f t="shared" si="11"/>
-        <v>24000</v>
-      </c>
-      <c r="AQ10" s="20">
-        <f t="shared" si="22"/>
-        <v>1.0439320000000001</v>
-      </c>
-      <c r="AR10" s="2"/>
+      <c r="AW10" s="2"/>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B11" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B11" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C11" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D11" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -2754,130 +2887,141 @@
         <v>56</v>
       </c>
       <c r="L11" s="1" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Junio</v>
-      </c>
-      <c r="M11" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="4">
         <v>1.3</v>
       </c>
-      <c r="N11" s="5">
+      <c r="O11" s="5">
         <v>10000</v>
       </c>
-      <c r="O11" s="5">
+      <c r="P11" s="5">
+        <f t="shared" si="12"/>
+        <v>13000</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y11" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z11" s="14">
+        <f>COUNTIFS($F$1:F11,F11,$K$1:K11,K11)+1</f>
+        <v>2</v>
+      </c>
+      <c r="AA11" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+      <c r="AB11" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>10000.00</v>
+      </c>
+      <c r="AC11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000</v>
+      </c>
+      <c r="AD11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>00000000</v>
+      </c>
+      <c r="AE11" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="13">
+        <f t="shared" si="4"/>
+        <v>2256.1999999999998</v>
+      </c>
+      <c r="AG11" s="13">
         <f t="shared" si="16"/>
         <v>13000</v>
       </c>
-      <c r="P11" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="14">
-        <f>COUNTIFS($F$1:F11,F11,$K$1:K11,K11)+1</f>
-        <v>2</v>
-      </c>
-      <c r="V11" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>1.3</v>
-      </c>
-      <c r="W11" s="18" t="str">
-        <f t="shared" si="17"/>
-        <v>10000.00</v>
-      </c>
-      <c r="X11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>00000</v>
-      </c>
-      <c r="Y11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z11" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA11" s="13">
-        <f t="shared" si="3"/>
-        <v>2256.1999999999998</v>
-      </c>
-      <c r="AB11" s="13">
+      <c r="AH11" s="10" t="str">
+        <f>IF(RIGHT(F11,1)="A",SUBSTITUTE(TEXT(P11,"0,00"),",","."),SUBSTITUTE(TEXT(AG11,"0,00"),",","."))</f>
+        <v>13000.00</v>
+      </c>
+      <c r="AI11" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>13000</v>
-      </c>
-      <c r="AC11" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>13000.00</v>
-      </c>
-      <c r="AD11" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1">
+        <f>ROW(K11)</f>
         <v>11</v>
       </c>
-      <c r="AG11" s="15" t="str">
+      <c r="AL11" s="15" t="str">
         <f>J11&amp;"-"&amp;COUNTIF($J$1:J11,J11)</f>
         <v>37473042-1</v>
       </c>
-      <c r="AH11" s="1">
+      <c r="AM11" s="1">
+        <f>IF(K10=K11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AN11" s="1">
+        <f>IF(K11=K12,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO11" s="1" t="str">
+        <f>RIGHT(F11)</f>
+        <v>B</v>
+      </c>
+      <c r="AP11" s="1">
+        <f>IF(LEFT(F11,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="13">
+        <f>IF(RIGHT(F11,1)="A",ROUND(O11*N11*(1+Q11),2),AG11)</f>
+        <v>13000</v>
+      </c>
+      <c r="AS11" s="13">
+        <f t="shared" si="5"/>
+        <v>10743.8</v>
+      </c>
+      <c r="AT11" s="20">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AI11" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="AU11" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>B</v>
-      </c>
-      <c r="AK11" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL11" s="2"/>
-      <c r="AM11" s="13">
-        <f t="shared" si="21"/>
         <v>13000</v>
       </c>
-      <c r="AN11" s="13">
-        <f t="shared" si="9"/>
-        <v>10743.8</v>
-      </c>
-      <c r="AO11" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV11" s="20">
+        <f t="shared" si="17"/>
         <v>1.3</v>
       </c>
-      <c r="AP11" s="13">
-        <f t="shared" si="11"/>
-        <v>13000</v>
-      </c>
-      <c r="AQ11" s="20">
-        <f t="shared" si="22"/>
-        <v>1.3</v>
-      </c>
-      <c r="AR11" s="2"/>
+      <c r="AW11" s="2"/>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B12" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B12" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C12" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D12" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -2901,130 +3045,141 @@
         <v>60</v>
       </c>
       <c r="L12" s="1" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Junio</v>
-      </c>
-      <c r="M12" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="4">
         <v>1.2105263157894737</v>
       </c>
-      <c r="N12" s="5">
+      <c r="O12" s="5">
         <v>19000</v>
       </c>
-      <c r="O12" s="5">
+      <c r="P12" s="5">
+        <f t="shared" si="12"/>
+        <v>23000</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y12" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z12" s="14">
+        <f>COUNTIFS($F$1:F12,F12,$K$1:K12,K12)+1</f>
+        <v>2</v>
+      </c>
+      <c r="AA12" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>1.210526</v>
+      </c>
+      <c r="AB12" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AC12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000</v>
+      </c>
+      <c r="AD12" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>00000000</v>
+      </c>
+      <c r="AE12" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF12" s="13">
+        <f t="shared" si="4"/>
+        <v>3991.74</v>
+      </c>
+      <c r="AG12" s="13">
         <f t="shared" si="16"/>
         <v>23000</v>
       </c>
-      <c r="P12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="14">
-        <f>COUNTIFS($F$1:F12,F12,$K$1:K12,K12)+1</f>
-        <v>2</v>
-      </c>
-      <c r="V12" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>1.210526</v>
-      </c>
-      <c r="W12" s="18" t="str">
-        <f t="shared" si="17"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>00000</v>
-      </c>
-      <c r="Y12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z12" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA12" s="13">
-        <f t="shared" si="3"/>
-        <v>3991.74</v>
-      </c>
-      <c r="AB12" s="13">
+      <c r="AH12" s="10" t="str">
+        <f>IF(RIGHT(F12,1)="A",SUBSTITUTE(TEXT(P12,"0,00"),",","."),SUBSTITUTE(TEXT(AG12,"0,00"),",","."))</f>
+        <v>23000.00</v>
+      </c>
+      <c r="AI12" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>23000</v>
-      </c>
-      <c r="AC12" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>23000.00</v>
-      </c>
-      <c r="AD12" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE12" s="1"/>
-      <c r="AF12" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1">
+        <f>ROW(K12)</f>
         <v>12</v>
       </c>
-      <c r="AG12" s="15" t="str">
+      <c r="AL12" s="15" t="str">
         <f>J12&amp;"-"&amp;COUNTIF($J$1:J12,J12)</f>
         <v>30707354719-1</v>
       </c>
-      <c r="AH12" s="1">
+      <c r="AM12" s="1">
+        <f>IF(K11=K12,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN12" s="1">
+        <f>IF(K12=K13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO12" s="1" t="str">
+        <f>RIGHT(F12)</f>
+        <v>B</v>
+      </c>
+      <c r="AP12" s="1">
+        <f>IF(LEFT(F12,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="13">
+        <f>IF(RIGHT(F12,1)="A",ROUND(O12*N12*(1+Q12),2),AG12)</f>
+        <v>23000</v>
+      </c>
+      <c r="AS12" s="13">
+        <f t="shared" si="5"/>
+        <v>19008.259999999998</v>
+      </c>
+      <c r="AT12" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI12" s="1">
+        <v>1.2105263157894737</v>
+      </c>
+      <c r="AU12" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>B</v>
-      </c>
-      <c r="AK12" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL12" s="2"/>
-      <c r="AM12" s="13">
-        <f t="shared" si="21"/>
         <v>23000</v>
       </c>
-      <c r="AN12" s="13">
-        <f t="shared" si="9"/>
-        <v>19008.259999999998</v>
-      </c>
-      <c r="AO12" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV12" s="20">
+        <f t="shared" si="17"/>
         <v>1.2105263157894737</v>
       </c>
-      <c r="AP12" s="13">
-        <f t="shared" si="11"/>
-        <v>23000</v>
-      </c>
-      <c r="AQ12" s="20">
-        <f t="shared" si="22"/>
-        <v>1.2105263157894737</v>
-      </c>
-      <c r="AR12" s="2"/>
+      <c r="AW12" s="2"/>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B13" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B13" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C13" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D13" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -3046,128 +3201,139 @@
         <v>70</v>
       </c>
       <c r="L13" s="1" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Junio</v>
-      </c>
-      <c r="M13" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="4">
         <v>1.5</v>
       </c>
-      <c r="N13" s="5">
+      <c r="O13" s="5">
         <v>19000</v>
       </c>
-      <c r="O13" s="5">
-        <f t="shared" si="16"/>
+      <c r="P13" s="5">
+        <f t="shared" si="12"/>
         <v>28500</v>
       </c>
-      <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="14">
+      <c r="T13" s="11"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y13" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z13" s="14">
         <f>COUNTIFS($F$1:F13,F13,$K$1:K13,K13)+1</f>
         <v>2</v>
       </c>
-      <c r="V13" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA13" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="W13" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB13" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X13" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC13" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y13" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD13" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z13" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA13" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="13">
+      <c r="AE13" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF13" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG13" s="13">
+        <f t="shared" si="16"/>
+        <v>28500</v>
+      </c>
+      <c r="AH13" s="10" t="str">
+        <f>IF(RIGHT(F13,1)="A",SUBSTITUTE(TEXT(P13,"0,00"),",","."),SUBSTITUTE(TEXT(AG13,"0,00"),",","."))</f>
+        <v>28500.00</v>
+      </c>
+      <c r="AI13" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>28500</v>
-      </c>
-      <c r="AC13" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>28500.00</v>
-      </c>
-      <c r="AD13" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1">
+        <f>ROW(K13)</f>
         <v>13</v>
       </c>
-      <c r="AG13" s="15" t="str">
+      <c r="AL13" s="15" t="str">
         <f>J13&amp;"-"&amp;COUNTIF($J$1:J13,J13)</f>
         <v>-0</v>
       </c>
-      <c r="AH13" s="1">
+      <c r="AM13" s="1">
+        <f>IF(K12=K13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN13" s="1">
+        <f>IF(K13=K14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO13" s="1" t="str">
+        <f>RIGHT(F13)</f>
+        <v>C</v>
+      </c>
+      <c r="AP13" s="1">
+        <f>IF(LEFT(F13,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="13">
+        <f>IF(RIGHT(F13,1)="A",ROUND(O13*N13*(1+Q13),2),AG13)</f>
+        <v>28500</v>
+      </c>
+      <c r="AS13" s="13">
+        <f t="shared" si="5"/>
+        <v>28500</v>
+      </c>
+      <c r="AT13" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AU13" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>C</v>
-      </c>
-      <c r="AK13" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL13" s="2"/>
-      <c r="AM13" s="13">
-        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
-      <c r="AN13" s="13">
-        <f t="shared" si="9"/>
-        <v>28500</v>
-      </c>
-      <c r="AO13" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV13" s="20">
+        <f t="shared" si="17"/>
         <v>1.5</v>
       </c>
-      <c r="AP13" s="13">
-        <f t="shared" si="11"/>
-        <v>28500</v>
-      </c>
-      <c r="AQ13" s="20">
-        <f t="shared" si="22"/>
-        <v>1.5</v>
-      </c>
-      <c r="AR13" s="2"/>
+      <c r="AW13" s="2"/>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B14" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B14" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C14" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D14" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
@@ -3193,135 +3359,146 @@
       <c r="L14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="2"/>
+      <c r="N14" s="4">
         <v>7.0247929999999998</v>
       </c>
-      <c r="N14" s="5">
+      <c r="O14" s="5">
         <v>19000</v>
       </c>
-      <c r="O14" s="5">
-        <f t="shared" si="16"/>
+      <c r="P14" s="5">
+        <f t="shared" si="12"/>
         <v>133471.06700000001</v>
       </c>
-      <c r="P14" s="11" t="s">
+      <c r="Q14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q14" s="11" t="s">
+      <c r="R14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="S14" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="S14" s="11" t="s">
+      <c r="T14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="T14" s="12">
+      <c r="U14" s="12">
         <v>44816</v>
       </c>
-      <c r="U14" s="14">
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y14" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z14" s="14">
         <f>COUNTIFS($F$1:F14,F14,$K$1:K14,K14)+1</f>
         <v>2</v>
       </c>
-      <c r="V14" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA14" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>7.024793</v>
       </c>
-      <c r="W14" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB14" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X14" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC14" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00002</v>
       </c>
-      <c r="Y14" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD14" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000150</v>
       </c>
-      <c r="Z14" s="9">
-        <f t="shared" si="18"/>
+      <c r="AE14" s="9">
+        <f t="shared" si="15"/>
         <v>44816</v>
       </c>
-      <c r="AA14" s="13">
-        <f t="shared" si="3"/>
+      <c r="AF14" s="13">
+        <f t="shared" si="4"/>
         <v>28028.92</v>
       </c>
-      <c r="AB14" s="13">
+      <c r="AG14" s="13">
+        <f t="shared" si="16"/>
+        <v>161499.99</v>
+      </c>
+      <c r="AH14" s="10" t="str">
+        <f>IF(RIGHT(F14,1)="A",SUBSTITUTE(TEXT(P14,"0,00"),",","."),SUBSTITUTE(TEXT(AG14,"0,00"),",","."))</f>
+        <v>133471.07</v>
+      </c>
+      <c r="AI14" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>161499.99</v>
-      </c>
-      <c r="AC14" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>133471.07</v>
-      </c>
-      <c r="AD14" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1">
+        <f>ROW(K14)</f>
         <v>14</v>
       </c>
-      <c r="AG14" s="15" t="str">
+      <c r="AL14" s="15" t="str">
         <f>J14&amp;"-"&amp;COUNTIF($J$1:J14,J14)</f>
         <v>30684125792-1</v>
       </c>
-      <c r="AH14" s="1">
+      <c r="AM14" s="1">
+        <f>IF(K13=K14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN14" s="1">
+        <f>IF(K14=K15,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO14" s="1" t="str">
+        <f>RIGHT(F14)</f>
+        <v>A</v>
+      </c>
+      <c r="AP14" s="1">
+        <f>IF(LEFT(F14,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="13">
+        <f>IF(RIGHT(F14,1)="A",ROUND(O14*N14*(1+Q14),2),AG14)</f>
+        <v>161499.99</v>
+      </c>
+      <c r="AS14" s="13">
+        <f t="shared" si="5"/>
+        <v>133471.07</v>
+      </c>
+      <c r="AT14" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI14" s="1">
+        <v>7.0247929999999998</v>
+      </c>
+      <c r="AU14" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK14" s="1">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AL14" s="2"/>
-      <c r="AM14" s="13">
-        <f t="shared" si="21"/>
-        <v>161499.99</v>
-      </c>
-      <c r="AN14" s="13">
-        <f t="shared" si="9"/>
-        <v>133471.07</v>
-      </c>
-      <c r="AO14" s="20">
-        <f t="shared" si="10"/>
+        <v>161500</v>
+      </c>
+      <c r="AV14" s="20">
+        <f t="shared" si="17"/>
         <v>7.0247929999999998</v>
       </c>
-      <c r="AP14" s="13">
-        <f t="shared" si="11"/>
-        <v>161500</v>
-      </c>
-      <c r="AQ14" s="20">
-        <f t="shared" si="22"/>
-        <v>7.0247929999999998</v>
-      </c>
-      <c r="AR14" s="2"/>
+      <c r="AW14" s="2"/>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B15" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B15" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C15" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D15" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -3347,135 +3524,146 @@
       <c r="L15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="2"/>
+      <c r="N15" s="4">
         <v>1.5</v>
       </c>
-      <c r="N15" s="5">
+      <c r="O15" s="5">
         <v>19000</v>
       </c>
-      <c r="O15" s="5">
+      <c r="P15" s="5">
+        <f t="shared" si="12"/>
+        <v>28500</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="U15" s="12">
+        <v>44816</v>
+      </c>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y15" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z15" s="14">
+        <f>COUNTIFS($F$1:F15,F15,$K$1:K15,K15)+1</f>
+        <v>2</v>
+      </c>
+      <c r="AA15" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="AB15" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AC15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00002</v>
+      </c>
+      <c r="AD15" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>00000152</v>
+      </c>
+      <c r="AE15" s="9">
+        <f t="shared" si="15"/>
+        <v>44816</v>
+      </c>
+      <c r="AF15" s="13">
+        <f t="shared" si="4"/>
+        <v>4946.28</v>
+      </c>
+      <c r="AG15" s="13">
         <f t="shared" si="16"/>
         <v>28500</v>
       </c>
-      <c r="P15" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q15" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="R15" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S15" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="T15" s="12">
-        <v>44816</v>
-      </c>
-      <c r="U15" s="14">
-        <f>COUNTIFS($F$1:F15,F15,$K$1:K15,K15)+1</f>
-        <v>2</v>
-      </c>
-      <c r="V15" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="W15" s="18" t="str">
-        <f t="shared" si="17"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>00002</v>
-      </c>
-      <c r="Y15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000152</v>
-      </c>
-      <c r="Z15" s="9">
-        <f t="shared" si="18"/>
-        <v>44816</v>
-      </c>
-      <c r="AA15" s="13">
-        <f t="shared" si="3"/>
-        <v>4946.28</v>
-      </c>
-      <c r="AB15" s="13">
+      <c r="AH15" s="10" t="str">
+        <f>IF(RIGHT(F15,1)="A",SUBSTITUTE(TEXT(P15,"0,00"),",","."),SUBSTITUTE(TEXT(AG15,"0,00"),",","."))</f>
+        <v>28500.00</v>
+      </c>
+      <c r="AI15" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>28500</v>
-      </c>
-      <c r="AC15" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>28500.00</v>
-      </c>
-      <c r="AD15" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE15" s="1"/>
-      <c r="AF15" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1">
+        <f>ROW(K15)</f>
         <v>15</v>
       </c>
-      <c r="AG15" s="15" t="str">
+      <c r="AL15" s="15" t="str">
         <f>J15&amp;"-"&amp;COUNTIF($J$1:J15,J15)</f>
         <v>30707354719-2</v>
       </c>
-      <c r="AH15" s="1">
+      <c r="AM15" s="1">
+        <f>IF(K14=K15,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN15" s="1">
+        <f>IF(K15=K16,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO15" s="1" t="str">
+        <f>RIGHT(F15)</f>
+        <v>B</v>
+      </c>
+      <c r="AP15" s="1">
+        <f>IF(LEFT(F15,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="13">
+        <f>IF(RIGHT(F15,1)="A",ROUND(O15*N15*(1+Q15),2),AG15)</f>
+        <v>28500</v>
+      </c>
+      <c r="AS15" s="13">
+        <f t="shared" si="5"/>
+        <v>23553.72</v>
+      </c>
+      <c r="AT15" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI15" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AU15" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>B</v>
-      </c>
-      <c r="AK15" s="1">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AL15" s="2"/>
-      <c r="AM15" s="13">
-        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
-      <c r="AN15" s="13">
-        <f t="shared" si="9"/>
-        <v>23553.72</v>
-      </c>
-      <c r="AO15" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV15" s="20">
+        <f t="shared" si="17"/>
         <v>1.5</v>
       </c>
-      <c r="AP15" s="13">
-        <f t="shared" si="11"/>
-        <v>28500</v>
-      </c>
-      <c r="AQ15" s="20">
-        <f t="shared" si="22"/>
-        <v>1.5</v>
-      </c>
-      <c r="AR15" s="2"/>
+      <c r="AW15" s="2"/>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B16" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B16" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C16" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D16" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -3501,135 +3689,146 @@
       <c r="L16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="2"/>
+      <c r="N16" s="4">
         <v>7.003044</v>
       </c>
-      <c r="N16" s="5">
+      <c r="O16" s="5">
         <v>19000</v>
       </c>
-      <c r="O16" s="5">
-        <f t="shared" si="16"/>
+      <c r="P16" s="5">
+        <f t="shared" si="12"/>
         <v>133057.83600000001</v>
       </c>
-      <c r="P16" s="11" t="s">
+      <c r="Q16" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="R16" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="S16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="S16" s="11" t="s">
+      <c r="T16" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="T16" s="12">
+      <c r="U16" s="12">
         <v>44816</v>
       </c>
-      <c r="U16" s="14">
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y16" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z16" s="14">
         <f>COUNTIFS($F$1:F16,F16,$K$1:K16,K16)+1</f>
         <v>2</v>
       </c>
-      <c r="V16" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA16" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>7.003044</v>
       </c>
-      <c r="W16" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB16" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X16" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC16" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00002</v>
       </c>
-      <c r="Y16" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD16" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000151</v>
       </c>
-      <c r="Z16" s="9">
-        <f t="shared" si="18"/>
+      <c r="AE16" s="9">
+        <f t="shared" si="15"/>
         <v>44816</v>
       </c>
-      <c r="AA16" s="13">
-        <f t="shared" si="3"/>
+      <c r="AF16" s="13">
+        <f t="shared" si="4"/>
         <v>27942.15</v>
       </c>
-      <c r="AB16" s="13">
+      <c r="AG16" s="13">
+        <f t="shared" si="16"/>
+        <v>160999.99</v>
+      </c>
+      <c r="AH16" s="10" t="str">
+        <f>IF(RIGHT(F16,1)="A",SUBSTITUTE(TEXT(P16,"0,00"),",","."),SUBSTITUTE(TEXT(AG16,"0,00"),",","."))</f>
+        <v>133057.84</v>
+      </c>
+      <c r="AI16" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>160999.99</v>
-      </c>
-      <c r="AC16" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>133057.84</v>
-      </c>
-      <c r="AD16" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1">
+        <f>ROW(K16)</f>
         <v>16</v>
       </c>
-      <c r="AG16" s="15" t="str">
+      <c r="AL16" s="15" t="str">
         <f>J16&amp;"-"&amp;COUNTIF($J$1:J16,J16)</f>
         <v>30684125792-2</v>
       </c>
-      <c r="AH16" s="1">
+      <c r="AM16" s="1">
+        <f>IF(K15=K16,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN16" s="1">
+        <f>IF(K16=K17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO16" s="1" t="str">
+        <f>RIGHT(F16)</f>
+        <v>A</v>
+      </c>
+      <c r="AP16" s="1">
+        <f>IF(LEFT(F16,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="13">
+        <f>IF(RIGHT(F16,1)="A",ROUND(O16*N16*(1+Q16),2),AG16)</f>
+        <v>160999.98000000001</v>
+      </c>
+      <c r="AS16" s="13">
+        <f t="shared" si="5"/>
+        <v>133057.82999999999</v>
+      </c>
+      <c r="AT16" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI16" s="1">
+        <v>7.003044</v>
+      </c>
+      <c r="AU16" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK16" s="1">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AL16" s="2"/>
-      <c r="AM16" s="13">
-        <f t="shared" si="21"/>
-        <v>160999.98000000001</v>
-      </c>
-      <c r="AN16" s="13">
-        <f t="shared" si="9"/>
-        <v>133057.82999999999</v>
-      </c>
-      <c r="AO16" s="20">
-        <f t="shared" si="10"/>
+        <v>161000</v>
+      </c>
+      <c r="AV16" s="20">
+        <f t="shared" si="17"/>
         <v>7.003044</v>
       </c>
-      <c r="AP16" s="13">
-        <f t="shared" si="11"/>
-        <v>161000</v>
-      </c>
-      <c r="AQ16" s="20">
-        <f t="shared" si="22"/>
-        <v>7.003044</v>
-      </c>
-      <c r="AR16" s="2"/>
+      <c r="AW16" s="2"/>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
+      </c>
+      <c r="B17" s="9">
+        <f t="shared" ca="1" si="9"/>
         <v>45108</v>
       </c>
-      <c r="B17" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45078</v>
-      </c>
       <c r="C17" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D17" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45122</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -3655,122 +3854,133 @@
       <c r="L17" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="2"/>
+      <c r="N17" s="4">
         <v>1.5</v>
       </c>
-      <c r="N17" s="5">
+      <c r="O17" s="5">
         <v>19000</v>
       </c>
-      <c r="O17" s="5">
+      <c r="P17" s="5">
+        <f t="shared" si="12"/>
+        <v>28500</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="S17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="U17" s="12">
+        <v>44816</v>
+      </c>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y17" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z17" s="14">
+        <f>COUNTIFS($F$1:F17,F17,$K$1:K17,K17)+1</f>
+        <v>2</v>
+      </c>
+      <c r="AA17" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="AB17" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AC17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00002</v>
+      </c>
+      <c r="AD17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>00000153</v>
+      </c>
+      <c r="AE17" s="9">
+        <f t="shared" si="15"/>
+        <v>44816</v>
+      </c>
+      <c r="AF17" s="13">
+        <f t="shared" si="4"/>
+        <v>4946.28</v>
+      </c>
+      <c r="AG17" s="13">
         <f t="shared" si="16"/>
         <v>28500</v>
       </c>
-      <c r="P17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q17" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="R17" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S17" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="T17" s="12">
-        <v>44816</v>
-      </c>
-      <c r="U17" s="14">
-        <f>COUNTIFS($F$1:F17,F17,$K$1:K17,K17)+1</f>
-        <v>2</v>
-      </c>
-      <c r="V17" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="W17" s="18" t="str">
-        <f t="shared" si="17"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>00002</v>
-      </c>
-      <c r="Y17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000153</v>
-      </c>
-      <c r="Z17" s="9">
-        <f t="shared" si="18"/>
-        <v>44816</v>
-      </c>
-      <c r="AA17" s="13">
-        <f t="shared" si="3"/>
-        <v>4946.28</v>
-      </c>
-      <c r="AB17" s="13">
+      <c r="AH17" s="10" t="str">
+        <f>IF(RIGHT(F17,1)="A",SUBSTITUTE(TEXT(P17,"0,00"),",","."),SUBSTITUTE(TEXT(AG17,"0,00"),",","."))</f>
+        <v>28500.00</v>
+      </c>
+      <c r="AI17" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>28500</v>
-      </c>
-      <c r="AC17" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>28500.00</v>
-      </c>
-      <c r="AD17" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE17" s="1"/>
-      <c r="AF17" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1">
+        <f>ROW(K17)</f>
         <v>17</v>
       </c>
-      <c r="AG17" s="15" t="str">
+      <c r="AL17" s="15" t="str">
         <f>J17&amp;"-"&amp;COUNTIF($J$1:J17,J17)</f>
         <v>37473042-2</v>
       </c>
-      <c r="AH17" s="1">
+      <c r="AM17" s="1">
+        <f>IF(K16=K17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN17" s="1">
+        <f>IF(K17=K18,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO17" s="1" t="str">
+        <f>RIGHT(F17)</f>
+        <v>B</v>
+      </c>
+      <c r="AP17" s="1">
+        <f>IF(LEFT(F17,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="13">
+        <f>IF(RIGHT(F17,1)="A",ROUND(O17*N17*(1+Q17),2),AG17)</f>
+        <v>28500</v>
+      </c>
+      <c r="AS17" s="13">
+        <f t="shared" si="5"/>
+        <v>23553.72</v>
+      </c>
+      <c r="AT17" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI17" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AU17" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>B</v>
-      </c>
-      <c r="AK17" s="1">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AL17" s="2"/>
-      <c r="AM17" s="13">
-        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
-      <c r="AN17" s="13">
-        <f t="shared" si="9"/>
-        <v>23553.72</v>
-      </c>
-      <c r="AO17" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV17" s="20">
+        <f t="shared" si="17"/>
         <v>1.5</v>
       </c>
-      <c r="AP17" s="13">
-        <f t="shared" si="11"/>
-        <v>28500</v>
-      </c>
-      <c r="AQ17" s="20">
-        <f t="shared" si="22"/>
-        <v>1.5</v>
-      </c>
-      <c r="AR17" s="2"/>
+      <c r="AW17" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AO17">
+  <autoFilter ref="A1:AU17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AT17">
     <sortCondition ref="F2:F17"/>
     <sortCondition ref="H2:H17"/>
     <sortCondition ref="J2:J17"/>

</xml_diff>

<commit_message>
Update excel and files
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808C8CFD-07D8-45CA-8342-D05B09214139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325D8F79-BB93-4A98-95BE-CE9A56432F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Factura" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AU$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AZ$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="94">
   <si>
     <t>Fecha</t>
   </si>
@@ -300,6 +300,24 @@
   </si>
   <si>
     <t>Bonif Facturador</t>
+  </si>
+  <si>
+    <t>Domicilio</t>
+  </si>
+  <si>
+    <t>Guardar</t>
+  </si>
+  <si>
+    <t>Ubicación a Guardar</t>
+  </si>
+  <si>
+    <t>C:\Users\ABP\Desktop\Test\</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -840,7 +858,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -865,7 +883,6 @@
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1228,12 +1245,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW17"/>
+  <dimension ref="A1:AZ17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AK1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1"/>
+      <selection pane="bottomLeft" activeCell="AY12" sqref="AY12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1289,7 @@
     <col min="46" max="46" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1420,11 +1437,20 @@
       <c r="AW1" s="19" t="s">
         <v>80</v>
       </c>
+      <c r="AX1" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f ca="1">TODAY()</f>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B2" s="9">
         <f ca="1">DATE(YEAR(C2),MONTH(C2),1)</f>
@@ -1436,7 +1462,7 @@
       </c>
       <c r="D2" s="9">
         <f ca="1">A2+14</f>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -1530,7 +1556,7 @@
         <f>SUBSTITUTE(TEXT(ROUNDUP(AG2,0)-AG2,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AJ2" s="22"/>
+      <c r="AJ2" s="2"/>
       <c r="AK2" s="1">
         <f t="shared" ref="AK2:AK17" si="6">ROW(K2)</f>
         <v>2</v>
@@ -1577,11 +1603,18 @@
         <v>7.003044</v>
       </c>
       <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f t="shared" ref="A3:A17" ca="1" si="15">TODAY()</f>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B3" s="9">
         <f t="shared" ref="B3:B17" ca="1" si="16">DATE(YEAR(C3),MONTH(C3),1)</f>
@@ -1593,7 +1626,7 @@
       </c>
       <c r="D3" s="9">
         <f t="shared" ref="D3:D17" ca="1" si="18">A3+14</f>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1688,7 +1721,7 @@
         <f>SUBSTITUTE(TEXT(ROUNDUP(AG3,0)-AG3,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AJ3" s="22"/>
+      <c r="AJ3" s="2"/>
       <c r="AK3" s="1">
         <f t="shared" si="6"/>
         <v>3</v>
@@ -1735,11 +1768,18 @@
         <v>8.0252280000000003</v>
       </c>
       <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B4" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -1751,7 +1791,7 @@
       </c>
       <c r="D4" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1846,7 +1886,7 @@
         <f>SUBSTITUTE(TEXT(ROUNDUP(AG4,0)-AG4,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
-      <c r="AJ4" s="22"/>
+      <c r="AJ4" s="2"/>
       <c r="AK4" s="1">
         <f t="shared" si="6"/>
         <v>4</v>
@@ -1893,11 +1933,18 @@
         <v>10.004348999999999</v>
       </c>
       <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B5" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -1909,7 +1956,7 @@
       </c>
       <c r="D5" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -2004,7 +2051,7 @@
         <f>SUBSTITUTE(TEXT(ROUNDUP(AG5,0)-AG5,"0,00"),",",".")</f>
         <v>0.00</v>
       </c>
-      <c r="AJ5" s="22"/>
+      <c r="AJ5" s="2"/>
       <c r="AK5" s="1">
         <f t="shared" si="6"/>
         <v>5</v>
@@ -2051,11 +2098,18 @@
         <v>9.0256629999999998</v>
       </c>
       <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B6" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2067,7 +2121,7 @@
       </c>
       <c r="D6" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -2170,7 +2224,7 @@
         <f>SUBSTITUTE(TEXT(ROUNDUP(AG6,0)-AG6,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AJ6" s="22"/>
+      <c r="AJ6" s="2"/>
       <c r="AK6" s="1">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -2217,11 +2271,18 @@
         <v>5.0239229999999999</v>
       </c>
       <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ6" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B7" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2233,7 +2294,7 @@
       </c>
       <c r="D7" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2327,7 +2388,7 @@
         <f t="shared" ref="AI7:AI17" si="26">SUBSTITUTE(TEXT(ROUNDUP(AG7,0)-AG7,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
-      <c r="AJ7" s="22"/>
+      <c r="AJ7" s="2"/>
       <c r="AK7" s="1">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -2374,11 +2435,18 @@
         <v>5.0021740000000001</v>
       </c>
       <c r="AW7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ7" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B8" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2390,7 +2458,7 @@
       </c>
       <c r="D8" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
@@ -2485,7 +2553,7 @@
         <f t="shared" si="26"/>
         <v>0.02</v>
       </c>
-      <c r="AJ8" s="22"/>
+      <c r="AJ8" s="2"/>
       <c r="AK8" s="1">
         <f t="shared" si="6"/>
         <v>8</v>
@@ -2532,11 +2600,18 @@
         <v>10.004348999999999</v>
       </c>
       <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ8" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B9" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2548,7 +2623,7 @@
       </c>
       <c r="D9" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -2643,7 +2718,7 @@
         <f t="shared" si="26"/>
         <v>0.01</v>
       </c>
-      <c r="AJ9" s="22"/>
+      <c r="AJ9" s="2"/>
       <c r="AK9" s="1">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -2690,11 +2765,18 @@
         <v>1.0221830000000001</v>
       </c>
       <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ9" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B10" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2706,7 +2788,7 @@
       </c>
       <c r="D10" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -2801,7 +2883,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ10" s="22"/>
+      <c r="AJ10" s="2"/>
       <c r="AK10" s="1">
         <f t="shared" si="6"/>
         <v>10</v>
@@ -2848,11 +2930,18 @@
         <v>1.0439320000000001</v>
       </c>
       <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ10" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B11" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2864,7 +2953,7 @@
       </c>
       <c r="D11" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -2959,7 +3048,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ11" s="22"/>
+      <c r="AJ11" s="2"/>
       <c r="AK11" s="1">
         <f t="shared" si="6"/>
         <v>11</v>
@@ -3006,11 +3095,16 @@
         <v>1.3</v>
       </c>
       <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ11" s="2"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B12" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3022,7 +3116,7 @@
       </c>
       <c r="D12" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -3117,7 +3211,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ12" s="22"/>
+      <c r="AJ12" s="2"/>
       <c r="AK12" s="1">
         <f t="shared" si="6"/>
         <v>12</v>
@@ -3164,11 +3258,16 @@
         <v>1.2105263157894737</v>
       </c>
       <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ12" s="2"/>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B13" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3180,7 +3279,7 @@
       </c>
       <c r="D13" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -3271,7 +3370,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ13" s="22"/>
+      <c r="AJ13" s="2"/>
       <c r="AK13" s="1">
         <f t="shared" si="6"/>
         <v>13</v>
@@ -3318,11 +3417,16 @@
         <v>1.5</v>
       </c>
       <c r="AW13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="AY13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ13" s="2"/>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B14" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3334,7 +3438,7 @@
       </c>
       <c r="D14" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
@@ -3436,7 +3540,7 @@
         <f t="shared" si="26"/>
         <v>0.01</v>
       </c>
-      <c r="AJ14" s="22"/>
+      <c r="AJ14" s="2"/>
       <c r="AK14" s="1">
         <f t="shared" si="6"/>
         <v>14</v>
@@ -3483,11 +3587,16 @@
         <v>7.0247929999999998</v>
       </c>
       <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ14" s="2"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B15" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3499,7 +3608,7 @@
       </c>
       <c r="D15" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -3601,7 +3710,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ15" s="22"/>
+      <c r="AJ15" s="2"/>
       <c r="AK15" s="1">
         <f t="shared" si="6"/>
         <v>15</v>
@@ -3648,11 +3757,16 @@
         <v>1.5</v>
       </c>
       <c r="AW15" s="2"/>
+      <c r="AX15" s="2"/>
+      <c r="AY15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ15" s="2"/>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B16" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3664,7 +3778,7 @@
       </c>
       <c r="D16" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -3766,7 +3880,7 @@
         <f t="shared" si="26"/>
         <v>0.01</v>
       </c>
-      <c r="AJ16" s="22"/>
+      <c r="AJ16" s="2"/>
       <c r="AK16" s="1">
         <f t="shared" si="6"/>
         <v>16</v>
@@ -3813,11 +3927,16 @@
         <v>7.003044</v>
       </c>
       <c r="AW16" s="2"/>
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ16" s="2"/>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B17" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3829,7 +3948,7 @@
       </c>
       <c r="D17" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -3931,7 +4050,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ17" s="22"/>
+      <c r="AJ17" s="2"/>
       <c r="AK17" s="1">
         <f t="shared" si="6"/>
         <v>17</v>
@@ -3978,14 +4097,24 @@
         <v>1.5</v>
       </c>
       <c r="AW17" s="2"/>
+      <c r="AX17" s="2"/>
+      <c r="AY17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ17" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AU17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AZ17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AT17">
     <sortCondition ref="F2:F17"/>
     <sortCondition ref="H2:H17"/>
     <sortCondition ref="J2:J17"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY17" xr:uid="{BFC33D16-50A8-46DB-B879-EC5A925DAA79}">
+      <formula1>"SI,NO"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
rename column 'Sin ST' for 'ST'
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Facturador-Multiusuario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Uipath\Facturador-Multiusuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99718EB-7D94-474D-8C38-325830975684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB5243C-711F-4911-BF86-AAF42ECF63AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Agustín Bustos:</t>
         </r>
@@ -59,7 +59,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Acá se pone el nombre a guardar de las facturas. Si se deja vacío se guarda con el nombre que define AFIP.</t>
@@ -74,7 +74,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Agustín Bustos:</t>
         </r>
@@ -83,10 +83,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Sin ST: SI: ejecutar cuando el bot no guarda los archivos con el nombre/ubicación definida</t>
+ST: NO: ejecutar cuando el bot no guarda los archivos con el nombre/ubicación definida</t>
         </r>
       </text>
     </comment>
@@ -98,7 +98,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Agustín Bustos:</t>
         </r>
@@ -107,7 +107,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Si se desae guardar el Archivo poner SI</t>
@@ -122,7 +122,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Agustín Bustos:</t>
         </r>
@@ -131,7 +131,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 la ubicación va desde el disco hasta la \final</t>
@@ -146,7 +146,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Agustín Bustos:</t>
         </r>
@@ -155,7 +155,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Se puede editar a necesidad de la empresa, en este caso factura a mes vencido</t>
@@ -170,7 +170,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Agustín Bustos:</t>
         </r>
@@ -179,7 +179,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Se puede editar a necesidad de la empresa, en este caso factura a mes vencido</t>
@@ -194,7 +194,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Agustín Bustos:</t>
         </r>
@@ -203,7 +203,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Si se deja vacío queda el default de AFIP. Ojo con CF que hay que identificar cuando supera el monto a informar</t>
@@ -218,7 +218,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Agustín Bustos:</t>
         </r>
@@ -227,7 +227,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Acá yo uso formulas porque generalmente facturo a mes vencido. Pero se pueden definir valores</t>
@@ -242,7 +242,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Agustín Bustos:</t>
         </r>
@@ -251,7 +251,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 si es factura C se deja vacío</t>
@@ -544,9 +544,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Sin ST</t>
-  </si>
-  <si>
     <t>Medio de Pago</t>
   </si>
   <si>
@@ -569,6 +566,9 @@
   </si>
   <si>
     <t>Otra</t>
+  </si>
+  <si>
+    <t>ST</t>
   </si>
 </sst>
 </file>
@@ -718,14 +718,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="37">
@@ -1122,7 +1122,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1147,7 +1147,6 @@
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1515,7 +1514,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,7 +1562,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>79</v>
@@ -1608,7 +1607,7 @@
         <v>10</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R1" s="16" t="s">
         <v>87</v>
@@ -1727,7 +1726,7 @@
       <c r="B2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
         <v>91</v>
       </c>
@@ -1736,19 +1735,19 @@
       </c>
       <c r="F2" s="8">
         <f ca="1">TODAY()</f>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G2" s="9">
         <f ca="1">DATE(YEAR(H2),MONTH(H2),1)</f>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H2" s="9">
         <f ca="1">EOMONTH(F2,-1)</f>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I2" s="9">
         <f ca="1">F2+14</f>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J2" s="2">
         <v>2</v>
@@ -1772,7 +1771,7 @@
         <v>52</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="6" t="s">
@@ -1894,12 +1893,12 @@
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2 - 30525733870 - PRICE WATERHOUSE &amp; CO SOCIEDAD DE RESPONSABILIDAD LIMITADA - Honorarios Julio</v>
+        <v>2 - 30525733870 - PRICE WATERHOUSE &amp; CO SOCIEDAD DE RESPONSABILIDAD LIMITADA - Honorarios Noviembre</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>91</v>
       </c>
@@ -1908,19 +1907,19 @@
       </c>
       <c r="F3" s="8">
         <f t="shared" ref="F3:F17" ca="1" si="20">TODAY()</f>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" ref="G3:G17" ca="1" si="21">DATE(YEAR(H3),MONTH(H3),1)</f>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H3" s="9">
         <f t="shared" ref="H3:H17" ca="1" si="22">EOMONTH(F3,-1)</f>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I3" s="9">
         <f t="shared" ref="I3:I17" ca="1" si="23">F3+14</f>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J3" s="2">
         <v>2</v>
@@ -1944,12 +1943,12 @@
         <v>49</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(G3,"mmmm"))</f>
-        <v>Honorarios Julio</v>
+        <v>Honorarios Noviembre</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="4">
@@ -2067,12 +2066,12 @@
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2 - 30610252334 - ARCOS DORADOS ARGENTINA SOCIEDAD ANONIMA - Honorarios Julio</v>
+        <v>2 - 30610252334 - ARCOS DORADOS ARGENTINA SOCIEDAD ANONIMA - Honorarios Noviembre</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>91</v>
       </c>
@@ -2081,19 +2080,19 @@
       </c>
       <c r="F4" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
@@ -2117,12 +2116,12 @@
         <v>41</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(G4,"mmmm"))</f>
-        <v>Honorarios Julio</v>
+        <v>Honorarios Noviembre</v>
       </c>
       <c r="T4" s="2"/>
       <c r="U4" s="4">
@@ -2240,12 +2239,12 @@
     <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2 - 30710964277 - LAKAUT S.A. - Honorarios Julio</v>
+        <v>2 - 30710964277 - LAKAUT S.A. - Honorarios Noviembre</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>91</v>
       </c>
@@ -2254,19 +2253,19 @@
       </c>
       <c r="F5" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G5" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J5" s="2">
         <v>2</v>
@@ -2290,12 +2289,12 @@
         <v>50</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(G5,"mmmm"))</f>
-        <v>Honorarios Julio</v>
+        <v>Honorarios Noviembre</v>
       </c>
       <c r="T5" s="2"/>
       <c r="U5" s="4">
@@ -2413,12 +2412,12 @@
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2 - 33610006189 - ACCENTURE SOCIEDAD DE RESPONSABILIDAD LIMITADA - Honorarios Julio</v>
+        <v>2 - 33610006189 - ACCENTURE SOCIEDAD DE RESPONSABILIDAD LIMITADA - Honorarios Noviembre</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>91</v>
       </c>
@@ -2427,19 +2426,19 @@
       </c>
       <c r="F6" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J6" s="2">
         <v>2</v>
@@ -2463,12 +2462,12 @@
         <v>36</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(G6,"mmmm"))</f>
-        <v>Honorarios Julio</v>
+        <v>Honorarios Noviembre</v>
       </c>
       <c r="T6" s="2"/>
       <c r="U6" s="4">
@@ -2599,7 +2598,7 @@
       <c r="B7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>91</v>
       </c>
@@ -2608,19 +2607,19 @@
       </c>
       <c r="F7" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J7" s="2">
         <v>2</v>
@@ -2644,7 +2643,7 @@
         <v>36</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R7" s="2"/>
       <c r="S7" s="6" t="s">
@@ -2766,12 +2765,12 @@
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2 - 33615420269 - AUSTRAL LINEAS AEREAS CIELOS DEL SUR S A - Honorarios Julio</v>
+        <v>2 - 33615420269 - AUSTRAL LINEAS AEREAS CIELOS DEL SUR S A - Honorarios Noviembre</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>91</v>
       </c>
@@ -2780,19 +2779,19 @@
       </c>
       <c r="F8" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G8" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H8" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I8" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J8" s="2">
         <v>2</v>
@@ -2816,12 +2815,12 @@
         <v>51</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="1" t="str">
         <f t="shared" ref="S8:S13" ca="1" si="30">"Honorarios "&amp;PROPER(TEXT(G8,"mmmm"))</f>
-        <v>Honorarios Julio</v>
+        <v>Honorarios Noviembre</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="4">
@@ -2939,12 +2938,12 @@
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2 - 20147130202 - BUSTOS JOSE MARTIN - Honorarios Julio</v>
+        <v>2 - 20147130202 - BUSTOS JOSE MARTIN - Honorarios Noviembre</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>91</v>
       </c>
@@ -2953,19 +2952,19 @@
       </c>
       <c r="F9" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G9" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H9" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I9" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J9" s="2">
         <v>2</v>
@@ -2989,12 +2988,12 @@
         <v>56</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="1" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>Honorarios Julio</v>
+        <v>Honorarios Noviembre</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="4">
@@ -3112,12 +3111,12 @@
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2 - 20374730429 - BUSTOS PIASENTINI AGUSTIN - Honorarios Julio</v>
+        <v>2 - 20374730429 - BUSTOS PIASENTINI AGUSTIN - Honorarios Noviembre</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>91</v>
       </c>
@@ -3126,19 +3125,19 @@
       </c>
       <c r="F10" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G10" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I10" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J10" s="2">
         <v>2</v>
@@ -3162,12 +3161,12 @@
         <v>55</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="1" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>Honorarios Julio</v>
+        <v>Honorarios Noviembre</v>
       </c>
       <c r="T10" s="2"/>
       <c r="U10" s="4">
@@ -3285,31 +3284,31 @@
     <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2 - 37473042 - BUSTOS PIASENTINI AGUSTIN - Honorarios Julio</v>
+        <v>2 - 37473042 - BUSTOS PIASENTINI AGUSTIN - Honorarios Noviembre</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G11" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H11" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I11" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J11" s="2">
         <v>2</v>
@@ -3333,12 +3332,12 @@
         <v>55</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="1" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>Honorarios Julio</v>
+        <v>Honorarios Noviembre</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="4">
@@ -3456,31 +3455,31 @@
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2 - 30707354719 - CAMARA DE ELABORADORES DE TE ARGENTINO C. E. T.A. - Honorarios Julio</v>
+        <v>2 - 30707354719 - CAMARA DE ELABORADORES DE TE ARGENTINO C. E. T.A. - Honorarios Noviembre</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G12" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J12" s="2">
         <v>2</v>
@@ -3504,12 +3503,12 @@
         <v>59</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="1" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>Honorarios Julio</v>
+        <v>Honorarios Noviembre</v>
       </c>
       <c r="T12" s="2"/>
       <c r="U12" s="4">
@@ -3627,31 +3626,31 @@
     <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>1 -  - MARTIN BUSTOS - Honorarios Julio</v>
+        <v>1 -  - MARTIN BUSTOS - Honorarios Noviembre</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G13" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I13" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
@@ -3673,12 +3672,12 @@
         <v>69</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="1" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>Honorarios Julio</v>
+        <v>Honorarios Noviembre</v>
       </c>
       <c r="T13" s="2"/>
       <c r="U13" s="4">
@@ -3799,26 +3798,26 @@
       <c r="B14" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G14" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I14" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J14" s="2">
         <v>2</v>
@@ -3842,7 +3841,7 @@
         <v>43</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="6" t="s">
@@ -3977,26 +3976,26 @@
       <c r="B15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G15" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H15" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I15" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J15" s="2">
         <v>2</v>
@@ -4020,7 +4019,7 @@
         <v>59</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="6" t="s">
@@ -4155,26 +4154,26 @@
       <c r="B16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="22"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G16" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H16" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I16" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J16" s="2">
         <v>2</v>
@@ -4198,7 +4197,7 @@
         <v>43</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="6" t="s">
@@ -4333,26 +4332,26 @@
       <c r="B17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="8">
         <f t="shared" ca="1" si="20"/>
-        <v>45149</v>
+        <v>45278</v>
       </c>
       <c r="G17" s="9">
         <f t="shared" ca="1" si="21"/>
-        <v>45108</v>
+        <v>45231</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" ca="1" si="22"/>
-        <v>45138</v>
+        <v>45260</v>
       </c>
       <c r="I17" s="9">
         <f t="shared" ca="1" si="23"/>
-        <v>45163</v>
+        <v>45292</v>
       </c>
       <c r="J17" s="2">
         <v>2</v>
@@ -4376,7 +4375,7 @@
         <v>55</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="6" t="s">
@@ -4546,37 +4545,37 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>